<commit_message>
SVN Revision #7105 by scriswellwsf       revisions to std design CathedralCeiling library objects (from BW) for MFam 2022+ analysis
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/shared/T24RClimateZoneCodeBaselines.xlsx
+++ b/RulesetDev/Rulesets/shared/T24RClimateZoneCodeBaselines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F05C2-0D86-46D9-B310-E560C6C8B5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2142204-AEBD-40AC-9B2F-2BA3D12E9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2175" windowWidth="24675" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12240" yWindow="2010" windowWidth="16215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T24RClimateZoneCodeBaselines" sheetId="1" r:id="rId1"/>
@@ -3120,13 +3120,13 @@
     <t>none</t>
   </si>
   <si>
-    <t>T24-22MF CathClg 2x12 R38 R1.1 U0.028</t>
+    <t>T24-22MF Framed Roof U=0.028</t>
   </si>
   <si>
-    <t>T24-22MF CathClg 2x10 R30 R0.8 U0.034</t>
+    <t>T24-22MF Framed Roof U=0.034</t>
   </si>
   <si>
-    <t>T24-22MF CathClg 2x10 R26 R0.2 U0.039</t>
+    <t>T24-22MF Framed Roof U=0.039</t>
   </si>
 </sst>
 </file>
@@ -4477,11 +4477,11 @@
   <dimension ref="A1:EY376"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C126" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="BF340" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="BH347" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C126" sqref="C126"/>
       <selection pane="topRight" activeCell="F126" sqref="F126"/>
       <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
-      <selection pane="bottomRight" activeCell="BH344" sqref="BH344"/>
+      <selection pane="bottomRight" activeCell="BH366" sqref="BH366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4534,7 +4534,7 @@
     <col min="57" max="57" width="33.42578125" customWidth="1"/>
     <col min="58" max="58" width="31.7109375" customWidth="1"/>
     <col min="59" max="59" width="33.140625" customWidth="1"/>
-    <col min="60" max="60" width="39.7109375" customWidth="1"/>
+    <col min="60" max="60" width="35.85546875" customWidth="1"/>
     <col min="61" max="61" width="11.7109375" customWidth="1"/>
     <col min="62" max="62" width="24.28515625" style="75" customWidth="1"/>
     <col min="63" max="63" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -59557,7 +59557,7 @@
       <c r="BG359" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="BH359" s="3" t="s">
+      <c r="BH359" s="84" t="s">
         <v>341</v>
       </c>
       <c r="BI359" s="19">

</xml_diff>

<commit_message>
SVN Revision #8146       Ticket #3455 MF Indirectly Conditioned Zones
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/shared/T24RClimateZoneCodeBaselines.xlsx
+++ b/RulesetDev/Rulesets/shared/T24RClimateZoneCodeBaselines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\360 Local\_CBECC Com MFamIndirectCondZn\RulesetDev\Rulesets\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51803EDA-A723-4BFF-B15B-8A70BC2FD5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFA1269-2898-45AA-9024-B16909BE4ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2715" windowWidth="25800" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="47565" windowHeight="19425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T24RClimateZoneCodeBaselines" sheetId="1" r:id="rId1"/>
@@ -2579,7 +2579,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9371" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9395" uniqueCount="398">
   <si>
     <t>;</t>
   </si>
@@ -5185,8 +5185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FM444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D429" sqref="D429"/>
+    <sheetView tabSelected="1" topLeftCell="AW391" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BJ420" sqref="BJ420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -79843,7 +79843,7 @@
         <v>374</v>
       </c>
       <c r="BJ412" s="2" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="BK412" s="2" t="s">
         <v>376</v>
@@ -80111,9 +80111,8 @@
       <c r="BI413" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ413" s="35" t="str">
-        <f>BJ412</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ413" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK413" s="2" t="s">
         <v>376</v>
@@ -80386,9 +80385,8 @@
       <c r="BI414" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ414" s="35" t="str">
-        <f t="shared" ref="BJ414:BJ427" si="890">BJ413</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ414" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK414" s="2" t="s">
         <v>376</v>
@@ -80436,23 +80434,23 @@
         <v>273</v>
       </c>
       <c r="BZ414" s="124" t="str">
-        <f t="shared" ref="BZ414:CD414" si="891">BZ413</f>
+        <f t="shared" ref="BZ414:CD414" si="890">BZ413</f>
         <v>not compact</v>
       </c>
       <c r="CA414" s="69" t="str">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>not compact</v>
       </c>
       <c r="CB414" s="35" t="str">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC414" s="35" t="str">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>Standard</v>
       </c>
       <c r="CD414" s="40">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>-1</v>
       </c>
       <c r="CE414" s="40">
@@ -80482,11 +80480,11 @@
         <v>4</v>
       </c>
       <c r="D415" s="35">
-        <f t="shared" ref="D415:E415" si="892">D414</f>
+        <f t="shared" ref="D415:E415" si="891">D414</f>
         <v>2025</v>
       </c>
       <c r="E415" s="40" t="str">
-        <f t="shared" si="892"/>
+        <f t="shared" si="891"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F415" s="2">
@@ -80596,11 +80594,11 @@
         <v>5016</v>
       </c>
       <c r="AO415" s="40">
-        <f t="shared" ref="AO415:AP415" si="893">AO414</f>
+        <f t="shared" ref="AO415:AP415" si="892">AO414</f>
         <v>0.7</v>
       </c>
       <c r="AP415" s="40" t="str">
-        <f t="shared" si="893"/>
+        <f t="shared" si="892"/>
         <v>Yes</v>
       </c>
       <c r="AQ415" s="138">
@@ -80661,9 +80659,8 @@
       <c r="BI415" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ415" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ415" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK415" s="2" t="s">
         <v>376</v>
@@ -80711,23 +80708,23 @@
         <v>274</v>
       </c>
       <c r="BZ415" s="124" t="str">
-        <f t="shared" ref="BZ415:CD415" si="894">BZ414</f>
+        <f t="shared" ref="BZ415:CD415" si="893">BZ414</f>
         <v>not compact</v>
       </c>
       <c r="CA415" s="69" t="str">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>not compact</v>
       </c>
       <c r="CB415" s="35" t="str">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC415" s="35" t="str">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>Standard</v>
       </c>
       <c r="CD415" s="40">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>-1</v>
       </c>
       <c r="CE415" s="40">
@@ -80757,11 +80754,11 @@
         <v>5</v>
       </c>
       <c r="D416" s="35">
-        <f t="shared" ref="D416:E416" si="895">D415</f>
+        <f t="shared" ref="D416:E416" si="894">D415</f>
         <v>2025</v>
       </c>
       <c r="E416" s="40" t="str">
-        <f t="shared" si="895"/>
+        <f t="shared" si="894"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F416" s="2">
@@ -80871,11 +80868,11 @@
         <v>5016</v>
       </c>
       <c r="AO416" s="40">
-        <f t="shared" ref="AO416:AP416" si="896">AO415</f>
+        <f t="shared" ref="AO416:AP416" si="895">AO415</f>
         <v>0.7</v>
       </c>
       <c r="AP416" s="40" t="str">
-        <f t="shared" si="896"/>
+        <f t="shared" si="895"/>
         <v>Yes</v>
       </c>
       <c r="AQ416" s="138">
@@ -80936,9 +80933,8 @@
       <c r="BI416" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ416" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ416" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK416" s="2" t="s">
         <v>376</v>
@@ -80986,23 +80982,23 @@
         <v>273</v>
       </c>
       <c r="BZ416" s="124" t="str">
-        <f t="shared" ref="BZ416:CD416" si="897">BZ415</f>
+        <f t="shared" ref="BZ416:CD416" si="896">BZ415</f>
         <v>not compact</v>
       </c>
       <c r="CA416" s="69" t="str">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>not compact</v>
       </c>
       <c r="CB416" s="35" t="str">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC416" s="35" t="str">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>Standard</v>
       </c>
       <c r="CD416" s="40">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>-1</v>
       </c>
       <c r="CE416" s="40">
@@ -81032,11 +81028,11 @@
         <v>6</v>
       </c>
       <c r="D417" s="35">
-        <f t="shared" ref="D417:E417" si="898">D416</f>
+        <f t="shared" ref="D417:E417" si="897">D416</f>
         <v>2025</v>
       </c>
       <c r="E417" s="40" t="str">
-        <f t="shared" si="898"/>
+        <f t="shared" si="897"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F417" s="2">
@@ -81146,11 +81142,11 @@
         <v>5016</v>
       </c>
       <c r="AO417" s="40">
-        <f t="shared" ref="AO417:AP419" si="899">AO416</f>
+        <f t="shared" ref="AO417:AP419" si="898">AO416</f>
         <v>0.7</v>
       </c>
       <c r="AP417" s="40" t="str">
-        <f t="shared" si="899"/>
+        <f t="shared" si="898"/>
         <v>Yes</v>
       </c>
       <c r="AQ417" s="138">
@@ -81212,7 +81208,7 @@
         <v>373</v>
       </c>
       <c r="BJ417" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK417" s="2" t="s">
         <v>376</v>
@@ -81260,23 +81256,23 @@
         <v>274</v>
       </c>
       <c r="BZ417" s="124" t="str">
-        <f t="shared" ref="BZ417:CD417" si="900">BZ416</f>
+        <f t="shared" ref="BZ417:CD417" si="899">BZ416</f>
         <v>not compact</v>
       </c>
       <c r="CA417" s="69" t="str">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>not compact</v>
       </c>
       <c r="CB417" s="35" t="str">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC417" s="35" t="str">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>Standard</v>
       </c>
       <c r="CD417" s="40">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>-1</v>
       </c>
       <c r="CE417" s="40">
@@ -81306,11 +81302,11 @@
         <v>7</v>
       </c>
       <c r="D418" s="35">
-        <f t="shared" ref="D418:E418" si="901">D417</f>
+        <f t="shared" ref="D418:E418" si="900">D417</f>
         <v>2025</v>
       </c>
       <c r="E418" s="40" t="str">
-        <f t="shared" si="901"/>
+        <f t="shared" si="900"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F418" s="2">
@@ -81420,7 +81416,7 @@
         <v>5016</v>
       </c>
       <c r="AO418" s="40">
-        <f t="shared" si="899"/>
+        <f t="shared" si="898"/>
         <v>0.7</v>
       </c>
       <c r="AP418" s="121" t="s">
@@ -81485,7 +81481,7 @@
         <v>373</v>
       </c>
       <c r="BJ418" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK418" s="2" t="s">
         <v>376</v>
@@ -81533,23 +81529,23 @@
         <v>274</v>
       </c>
       <c r="BZ418" s="124" t="str">
-        <f t="shared" ref="BZ418:CD418" si="902">BZ417</f>
+        <f t="shared" ref="BZ418:CD418" si="901">BZ417</f>
         <v>not compact</v>
       </c>
       <c r="CA418" s="69" t="str">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>not compact</v>
       </c>
       <c r="CB418" s="35" t="str">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC418" s="35" t="str">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>Standard</v>
       </c>
       <c r="CD418" s="40">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>-1</v>
       </c>
       <c r="CE418" s="40">
@@ -81579,11 +81575,11 @@
         <v>8</v>
       </c>
       <c r="D419" s="35">
-        <f t="shared" ref="D419:E419" si="903">D418</f>
+        <f t="shared" ref="D419:E419" si="902">D418</f>
         <v>2025</v>
       </c>
       <c r="E419" s="40" t="str">
-        <f t="shared" si="903"/>
+        <f t="shared" si="902"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F419" s="2">
@@ -81693,7 +81689,7 @@
         <v>5016</v>
       </c>
       <c r="AO419" s="40">
-        <f t="shared" si="899"/>
+        <f t="shared" si="898"/>
         <v>0.7</v>
       </c>
       <c r="AP419" s="38" t="s">
@@ -81758,7 +81754,7 @@
         <v>374</v>
       </c>
       <c r="BJ419" s="2" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="BK419" s="2" t="s">
         <v>376</v>
@@ -81806,23 +81802,23 @@
         <v>274</v>
       </c>
       <c r="BZ419" s="124" t="str">
-        <f t="shared" ref="BZ419:CD419" si="904">BZ418</f>
+        <f t="shared" ref="BZ419:CD419" si="903">BZ418</f>
         <v>not compact</v>
       </c>
       <c r="CA419" s="69" t="str">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>not compact</v>
       </c>
       <c r="CB419" s="35" t="str">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC419" s="35" t="str">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>Standard</v>
       </c>
       <c r="CD419" s="40">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>-1</v>
       </c>
       <c r="CE419" s="40">
@@ -81852,11 +81848,11 @@
         <v>9</v>
       </c>
       <c r="D420" s="35">
-        <f t="shared" ref="D420:E420" si="905">D419</f>
+        <f t="shared" ref="D420:E420" si="904">D419</f>
         <v>2025</v>
       </c>
       <c r="E420" s="40" t="str">
-        <f t="shared" si="905"/>
+        <f t="shared" si="904"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F420" s="2">
@@ -81966,11 +81962,11 @@
         <v>5016</v>
       </c>
       <c r="AO420" s="40">
-        <f t="shared" ref="AO420:AP420" si="906">AO419</f>
+        <f t="shared" ref="AO420:AP420" si="905">AO419</f>
         <v>0.7</v>
       </c>
       <c r="AP420" s="40" t="str">
-        <f t="shared" si="906"/>
+        <f t="shared" si="905"/>
         <v>Yes</v>
       </c>
       <c r="AQ420" s="138">
@@ -82031,9 +82027,8 @@
       <c r="BI420" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ420" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ420" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK420" s="2" t="s">
         <v>376</v>
@@ -82081,23 +82076,23 @@
         <v>274</v>
       </c>
       <c r="BZ420" s="124" t="str">
-        <f t="shared" ref="BZ420:CD420" si="907">BZ419</f>
+        <f t="shared" ref="BZ420:CD420" si="906">BZ419</f>
         <v>not compact</v>
       </c>
       <c r="CA420" s="69" t="str">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>not compact</v>
       </c>
       <c r="CB420" s="35" t="str">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC420" s="35" t="str">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>Standard</v>
       </c>
       <c r="CD420" s="40">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>-1</v>
       </c>
       <c r="CE420" s="40">
@@ -82127,11 +82122,11 @@
         <v>10</v>
       </c>
       <c r="D421" s="35">
-        <f t="shared" ref="D421:E421" si="908">D420</f>
+        <f t="shared" ref="D421:E421" si="907">D420</f>
         <v>2025</v>
       </c>
       <c r="E421" s="40" t="str">
-        <f t="shared" si="908"/>
+        <f t="shared" si="907"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F421" s="2">
@@ -82241,11 +82236,11 @@
         <v>5016</v>
       </c>
       <c r="AO421" s="40">
-        <f t="shared" ref="AO421:AP421" si="909">AO420</f>
+        <f t="shared" ref="AO421:AP421" si="908">AO420</f>
         <v>0.7</v>
       </c>
       <c r="AP421" s="40" t="str">
-        <f t="shared" si="909"/>
+        <f t="shared" si="908"/>
         <v>Yes</v>
       </c>
       <c r="AQ421" s="138">
@@ -82306,9 +82301,8 @@
       <c r="BI421" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ421" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ421" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK421" s="2" t="s">
         <v>376</v>
@@ -82356,23 +82350,23 @@
         <v>274</v>
       </c>
       <c r="BZ421" s="124" t="str">
-        <f t="shared" ref="BZ421:CD421" si="910">BZ420</f>
+        <f t="shared" ref="BZ421:CD421" si="909">BZ420</f>
         <v>not compact</v>
       </c>
       <c r="CA421" s="69" t="str">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>not compact</v>
       </c>
       <c r="CB421" s="35" t="str">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC421" s="35" t="str">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>Standard</v>
       </c>
       <c r="CD421" s="40">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>-1</v>
       </c>
       <c r="CE421" s="40">
@@ -82402,11 +82396,11 @@
         <v>11</v>
       </c>
       <c r="D422" s="35">
-        <f t="shared" ref="D422:E422" si="911">D421</f>
+        <f t="shared" ref="D422:E422" si="910">D421</f>
         <v>2025</v>
       </c>
       <c r="E422" s="40" t="str">
-        <f t="shared" si="911"/>
+        <f t="shared" si="910"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F422" s="2">
@@ -82516,11 +82510,11 @@
         <v>5016</v>
       </c>
       <c r="AO422" s="40">
-        <f t="shared" ref="AO422:AP422" si="912">AO421</f>
+        <f t="shared" ref="AO422:AP422" si="911">AO421</f>
         <v>0.7</v>
       </c>
       <c r="AP422" s="40" t="str">
-        <f t="shared" si="912"/>
+        <f t="shared" si="911"/>
         <v>Yes</v>
       </c>
       <c r="AQ422" s="138">
@@ -82581,9 +82575,8 @@
       <c r="BI422" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ422" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ422" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK422" s="2" t="s">
         <v>376</v>
@@ -82631,23 +82624,23 @@
         <v>274</v>
       </c>
       <c r="BZ422" s="124" t="str">
-        <f t="shared" ref="BZ422:CD422" si="913">BZ421</f>
+        <f t="shared" ref="BZ422:CD422" si="912">BZ421</f>
         <v>not compact</v>
       </c>
       <c r="CA422" s="69" t="str">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>not compact</v>
       </c>
       <c r="CB422" s="35" t="str">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC422" s="35" t="str">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>Standard</v>
       </c>
       <c r="CD422" s="40">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>-1</v>
       </c>
       <c r="CE422" s="40">
@@ -82677,11 +82670,11 @@
         <v>12</v>
       </c>
       <c r="D423" s="35">
-        <f t="shared" ref="D423:E423" si="914">D422</f>
+        <f t="shared" ref="D423:E423" si="913">D422</f>
         <v>2025</v>
       </c>
       <c r="E423" s="40" t="str">
-        <f t="shared" si="914"/>
+        <f t="shared" si="913"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F423" s="2">
@@ -82791,11 +82784,11 @@
         <v>5016</v>
       </c>
       <c r="AO423" s="40">
-        <f t="shared" ref="AO423:AP423" si="915">AO422</f>
+        <f t="shared" ref="AO423:AP423" si="914">AO422</f>
         <v>0.7</v>
       </c>
       <c r="AP423" s="40" t="str">
-        <f t="shared" si="915"/>
+        <f t="shared" si="914"/>
         <v>Yes</v>
       </c>
       <c r="AQ423" s="138">
@@ -82856,9 +82849,8 @@
       <c r="BI423" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ423" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ423" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK423" s="2" t="s">
         <v>376</v>
@@ -82906,23 +82898,23 @@
         <v>274</v>
       </c>
       <c r="BZ423" s="124" t="str">
-        <f t="shared" ref="BZ423:CD423" si="916">BZ422</f>
+        <f t="shared" ref="BZ423:CD423" si="915">BZ422</f>
         <v>not compact</v>
       </c>
       <c r="CA423" s="69" t="str">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>not compact</v>
       </c>
       <c r="CB423" s="35" t="str">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC423" s="35" t="str">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>Standard</v>
       </c>
       <c r="CD423" s="40">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>-1</v>
       </c>
       <c r="CE423" s="40">
@@ -82952,11 +82944,11 @@
         <v>13</v>
       </c>
       <c r="D424" s="35">
-        <f t="shared" ref="D424:E424" si="917">D423</f>
+        <f t="shared" ref="D424:E424" si="916">D423</f>
         <v>2025</v>
       </c>
       <c r="E424" s="40" t="str">
-        <f t="shared" si="917"/>
+        <f t="shared" si="916"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F424" s="2">
@@ -83066,11 +83058,11 @@
         <v>5016</v>
       </c>
       <c r="AO424" s="40">
-        <f t="shared" ref="AO424:AP424" si="918">AO423</f>
+        <f t="shared" ref="AO424:AP424" si="917">AO423</f>
         <v>0.7</v>
       </c>
       <c r="AP424" s="40" t="str">
-        <f t="shared" si="918"/>
+        <f t="shared" si="917"/>
         <v>Yes</v>
       </c>
       <c r="AQ424" s="138">
@@ -83131,9 +83123,8 @@
       <c r="BI424" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ424" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ424" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK424" s="2" t="s">
         <v>376</v>
@@ -83181,23 +83172,23 @@
         <v>274</v>
       </c>
       <c r="BZ424" s="124" t="str">
-        <f t="shared" ref="BZ424:CD424" si="919">BZ423</f>
+        <f t="shared" ref="BZ424:CD424" si="918">BZ423</f>
         <v>not compact</v>
       </c>
       <c r="CA424" s="69" t="str">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>not compact</v>
       </c>
       <c r="CB424" s="35" t="str">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC424" s="35" t="str">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>Standard</v>
       </c>
       <c r="CD424" s="40">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>-1</v>
       </c>
       <c r="CE424" s="40">
@@ -83227,11 +83218,11 @@
         <v>14</v>
       </c>
       <c r="D425" s="35">
-        <f t="shared" ref="D425:E425" si="920">D424</f>
+        <f t="shared" ref="D425:E425" si="919">D424</f>
         <v>2025</v>
       </c>
       <c r="E425" s="40" t="str">
-        <f t="shared" si="920"/>
+        <f t="shared" si="919"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F425" s="2">
@@ -83341,11 +83332,11 @@
         <v>5016</v>
       </c>
       <c r="AO425" s="40">
-        <f t="shared" ref="AO425:AP425" si="921">AO424</f>
+        <f t="shared" ref="AO425:AP425" si="920">AO424</f>
         <v>0.7</v>
       </c>
       <c r="AP425" s="40" t="str">
-        <f t="shared" si="921"/>
+        <f t="shared" si="920"/>
         <v>Yes</v>
       </c>
       <c r="AQ425" s="138">
@@ -83406,9 +83397,8 @@
       <c r="BI425" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ425" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ425" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK425" s="2" t="s">
         <v>376</v>
@@ -83456,23 +83446,23 @@
         <v>274</v>
       </c>
       <c r="BZ425" s="124" t="str">
-        <f t="shared" ref="BZ425:CD425" si="922">BZ424</f>
+        <f t="shared" ref="BZ425:CD425" si="921">BZ424</f>
         <v>not compact</v>
       </c>
       <c r="CA425" s="69" t="str">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>not compact</v>
       </c>
       <c r="CB425" s="35" t="str">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC425" s="35" t="str">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>Standard</v>
       </c>
       <c r="CD425" s="40">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>-1</v>
       </c>
       <c r="CE425" s="40">
@@ -83502,11 +83492,11 @@
         <v>15</v>
       </c>
       <c r="D426" s="35">
-        <f t="shared" ref="D426:E426" si="923">D425</f>
+        <f t="shared" ref="D426:E426" si="922">D425</f>
         <v>2025</v>
       </c>
       <c r="E426" s="40" t="str">
-        <f t="shared" si="923"/>
+        <f t="shared" si="922"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F426" s="2">
@@ -83616,11 +83606,11 @@
         <v>5016</v>
       </c>
       <c r="AO426" s="40">
-        <f t="shared" ref="AO426:AP426" si="924">AO425</f>
+        <f t="shared" ref="AO426:AP426" si="923">AO425</f>
         <v>0.7</v>
       </c>
       <c r="AP426" s="40" t="str">
-        <f t="shared" si="924"/>
+        <f t="shared" si="923"/>
         <v>Yes</v>
       </c>
       <c r="AQ426" s="138">
@@ -83681,9 +83671,8 @@
       <c r="BI426" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ426" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ426" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK426" s="2" t="s">
         <v>376</v>
@@ -83731,23 +83720,23 @@
         <v>274</v>
       </c>
       <c r="BZ426" s="124" t="str">
-        <f t="shared" ref="BZ426:CD426" si="925">BZ425</f>
+        <f t="shared" ref="BZ426:CD426" si="924">BZ425</f>
         <v>not compact</v>
       </c>
       <c r="CA426" s="69" t="str">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>not compact</v>
       </c>
       <c r="CB426" s="35" t="str">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC426" s="35" t="str">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>Standard</v>
       </c>
       <c r="CD426" s="40">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>-1</v>
       </c>
       <c r="CE426" s="40">
@@ -83777,11 +83766,11 @@
         <v>16</v>
       </c>
       <c r="D427" s="35">
-        <f t="shared" ref="D427:E427" si="926">D426</f>
+        <f t="shared" ref="D427:E427" si="925">D426</f>
         <v>2025</v>
       </c>
       <c r="E427" s="40" t="str">
-        <f t="shared" si="926"/>
+        <f t="shared" si="925"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F427" s="2">
@@ -83891,11 +83880,11 @@
         <v>10016</v>
       </c>
       <c r="AO427" s="40">
-        <f t="shared" ref="AO427:AP427" si="927">AO426</f>
+        <f t="shared" ref="AO427:AP427" si="926">AO426</f>
         <v>0.7</v>
       </c>
       <c r="AP427" s="40" t="str">
-        <f t="shared" si="927"/>
+        <f t="shared" si="926"/>
         <v>Yes</v>
       </c>
       <c r="AQ427" s="138">
@@ -83956,9 +83945,8 @@
       <c r="BI427" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ427" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ427" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK427" s="2" t="s">
         <v>375</v>
@@ -84006,23 +83994,23 @@
         <v>274</v>
       </c>
       <c r="BZ427" s="124" t="str">
-        <f t="shared" ref="BZ427:CD427" si="928">BZ426</f>
+        <f t="shared" ref="BZ427:CD427" si="927">BZ426</f>
         <v>not compact</v>
       </c>
       <c r="CA427" s="69" t="str">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>not compact</v>
       </c>
       <c r="CB427" s="35" t="str">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC427" s="35" t="str">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>Standard</v>
       </c>
       <c r="CD427" s="40">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>-1</v>
       </c>
       <c r="CE427" s="121">
@@ -84125,18 +84113,18 @@
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB428" s="140">
-        <f t="shared" ref="AB428:AB443" si="929">AB412</f>
+        <f t="shared" ref="AB428:AB443" si="928">AB412</f>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC428" s="144">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD428" s="144">
-        <f t="shared" ref="AD428:AE428" si="930">AD412</f>
+        <f t="shared" ref="AD428:AE428" si="929">AD412</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE428" s="144">
-        <f t="shared" si="930"/>
+        <f t="shared" si="929"/>
         <v>0.253</v>
       </c>
       <c r="AF428" s="140">
@@ -84229,22 +84217,22 @@
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH428" s="145" t="str">
-        <f t="shared" ref="BH428:BI428" si="931">BH412</f>
+        <f t="shared" ref="BH428:BI428" si="930">BH412</f>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI428" s="145" t="str">
+        <f t="shared" si="930"/>
+        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
+      </c>
+      <c r="BJ428" s="140" t="s">
+        <v>338</v>
+      </c>
+      <c r="BK428" s="145" t="str">
+        <f t="shared" ref="BK428:BL428" si="931">BK412</f>
+        <v>T24-2022 ExtWall 6in Conc R13</v>
+      </c>
+      <c r="BL428" s="145" t="str">
         <f t="shared" si="931"/>
-        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
-      </c>
-      <c r="BJ428" s="140" t="s">
-        <v>203</v>
-      </c>
-      <c r="BK428" s="145" t="str">
-        <f t="shared" ref="BK428:BL428" si="932">BK412</f>
-        <v>T24-2022 ExtWall 6in Conc R13</v>
-      </c>
-      <c r="BL428" s="145" t="str">
-        <f t="shared" si="932"/>
         <v>T24-2022 ExtWall 8in Conc U=0.253</v>
       </c>
       <c r="BM428" s="140" t="s">
@@ -84332,7 +84320,7 @@
         <v>2025</v>
       </c>
       <c r="E429" s="40" t="str">
-        <f t="shared" ref="E429" si="933">E428</f>
+        <f t="shared" ref="E429" si="932">E428</f>
         <v>HiRiseRes</v>
       </c>
       <c r="F429" s="2">
@@ -84400,22 +84388,22 @@
         <v>15</v>
       </c>
       <c r="AA429" s="2">
-        <f t="shared" ref="AA429:AA443" si="934">AA413</f>
+        <f t="shared" ref="AA429:AA443" si="933">AA413</f>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB429" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC429" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD429" s="120">
-        <f t="shared" ref="AD429:AE429" si="935">AD413</f>
+        <f t="shared" ref="AD429:AE429" si="934">AD413</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE429" s="120">
-        <f t="shared" si="935"/>
+        <f t="shared" si="934"/>
         <v>0.65</v>
       </c>
       <c r="AF429" s="2">
@@ -84507,27 +84495,26 @@
         <v>0</v>
       </c>
       <c r="BG429" s="138" t="str">
-        <f t="shared" ref="BG429:BI443" si="936">BG413</f>
+        <f t="shared" ref="BG429:BI443" si="935">BG413</f>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH429" s="138" t="str">
+        <f t="shared" si="935"/>
+        <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
+      </c>
+      <c r="BI429" s="138" t="str">
+        <f t="shared" si="935"/>
+        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
+      </c>
+      <c r="BJ429" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="BK429" s="138" t="str">
+        <f t="shared" ref="BK429:BL429" si="936">BK413</f>
+        <v>T24-2022 ExtWall 6in Conc R13</v>
+      </c>
+      <c r="BL429" s="138" t="str">
         <f t="shared" si="936"/>
-        <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
-      </c>
-      <c r="BI429" s="138" t="str">
-        <f t="shared" si="936"/>
-        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
-      </c>
-      <c r="BJ429" s="35" t="str">
-        <f>BJ428</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
-      </c>
-      <c r="BK429" s="138" t="str">
-        <f t="shared" ref="BK429:BL429" si="937">BK413</f>
-        <v>T24-2022 ExtWall 6in Conc R13</v>
-      </c>
-      <c r="BL429" s="138" t="str">
-        <f t="shared" si="937"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM429" s="2" t="s">
@@ -84616,11 +84603,11 @@
         <v>3</v>
       </c>
       <c r="D430" s="35">
-        <f t="shared" ref="D430:E430" si="938">D429</f>
+        <f t="shared" ref="D430:E430" si="937">D429</f>
         <v>2025</v>
       </c>
       <c r="E430" s="40" t="str">
-        <f t="shared" si="938"/>
+        <f t="shared" si="937"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F430" s="2">
@@ -84666,7 +84653,7 @@
         <v>0.62</v>
       </c>
       <c r="T430" s="35">
-        <f t="shared" ref="T430:T443" si="939">T429</f>
+        <f t="shared" ref="T430:T443" si="938">T429</f>
         <v>7</v>
       </c>
       <c r="U430" s="38">
@@ -84688,22 +84675,22 @@
         <v>15</v>
       </c>
       <c r="AA430" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB430" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC430" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD430" s="120">
-        <f t="shared" ref="AD430:AE430" si="940">AD414</f>
+        <f t="shared" ref="AD430:AE430" si="939">AD414</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE430" s="120">
-        <f t="shared" si="940"/>
+        <f t="shared" si="939"/>
         <v>0.65</v>
       </c>
       <c r="AF430" s="2">
@@ -84734,33 +84721,33 @@
         <v>5016</v>
       </c>
       <c r="AO430" s="40">
-        <f t="shared" ref="AO430:AP430" si="941">AO429</f>
+        <f t="shared" ref="AO430:AP430" si="940">AO429</f>
         <v>0.7</v>
       </c>
       <c r="AP430" s="40" t="str">
-        <f t="shared" si="941"/>
+        <f t="shared" si="940"/>
         <v>Yes</v>
       </c>
       <c r="AQ430" s="138">
-        <f t="shared" ref="AQ430:AS430" si="942">AQ414</f>
+        <f t="shared" ref="AQ430" si="941">AQ414</f>
         <v>0.41</v>
       </c>
       <c r="AR430" s="138">
         <v>0.26</v>
       </c>
       <c r="AS430" s="138">
-        <f t="shared" ref="AS430:AU443" si="943">AS414</f>
+        <f t="shared" ref="AS430:AT443" si="942">AS414</f>
         <v>0.46</v>
       </c>
       <c r="AT430" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU430" s="138">
         <v>0.24</v>
       </c>
       <c r="AV430" s="138">
-        <f t="shared" ref="AV430:AV443" si="944">AV414</f>
+        <f t="shared" ref="AV430:AV443" si="943">AV414</f>
         <v>0.37</v>
       </c>
       <c r="AW430" s="38">
@@ -84791,31 +84778,30 @@
         <v>114</v>
       </c>
       <c r="BF430" s="40">
-        <f t="shared" ref="BF430:BF443" si="945">BF429</f>
+        <f t="shared" ref="BF430:BF443" si="944">BF429</f>
         <v>0</v>
       </c>
       <c r="BG430" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH430" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI430" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ430" s="35" t="str">
-        <f t="shared" ref="BJ430:BJ443" si="946">BJ429</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ430" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK430" s="138" t="str">
-        <f t="shared" ref="BK430:BL430" si="947">BK414</f>
+        <f t="shared" ref="BK430:BL430" si="945">BK414</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL430" s="138" t="str">
-        <f t="shared" si="947"/>
+        <f t="shared" si="945"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM430" s="2" t="s">
@@ -84858,23 +84844,23 @@
         <v>273</v>
       </c>
       <c r="BZ430" s="124" t="str">
-        <f t="shared" ref="BZ430:CD430" si="948">BZ429</f>
+        <f t="shared" ref="BZ430:CD430" si="946">BZ429</f>
         <v>not compact</v>
       </c>
       <c r="CA430" s="69" t="str">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>not compact</v>
       </c>
       <c r="CB430" s="35" t="str">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC430" s="35" t="str">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>Standard</v>
       </c>
       <c r="CD430" s="40">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>-1</v>
       </c>
       <c r="CE430" s="40">
@@ -84904,11 +84890,11 @@
         <v>4</v>
       </c>
       <c r="D431" s="35">
-        <f t="shared" ref="D431:E431" si="949">D430</f>
+        <f t="shared" ref="D431:E431" si="947">D430</f>
         <v>2025</v>
       </c>
       <c r="E431" s="40" t="str">
-        <f t="shared" si="949"/>
+        <f t="shared" si="947"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F431" s="2">
@@ -84954,7 +84940,7 @@
         <v>0.62</v>
       </c>
       <c r="T431" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U431" s="38">
@@ -84976,22 +84962,22 @@
         <v>15</v>
       </c>
       <c r="AA431" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB431" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC431" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD431" s="120">
-        <f t="shared" ref="AD431:AE431" si="950">AD415</f>
+        <f t="shared" ref="AD431:AE431" si="948">AD415</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE431" s="120">
-        <f t="shared" si="950"/>
+        <f t="shared" si="948"/>
         <v>0.65</v>
       </c>
       <c r="AF431" s="2">
@@ -85022,33 +85008,33 @@
         <v>5016</v>
       </c>
       <c r="AO431" s="40">
-        <f t="shared" ref="AO431:AP431" si="951">AO430</f>
+        <f t="shared" ref="AO431:AP431" si="949">AO430</f>
         <v>0.7</v>
       </c>
       <c r="AP431" s="40" t="str">
-        <f t="shared" si="951"/>
+        <f t="shared" si="949"/>
         <v>Yes</v>
       </c>
       <c r="AQ431" s="138">
-        <f t="shared" ref="AQ431:AS431" si="952">AQ415</f>
+        <f t="shared" ref="AQ431" si="950">AQ415</f>
         <v>0.41</v>
       </c>
       <c r="AR431" s="138">
         <v>0.26</v>
       </c>
       <c r="AS431" s="138">
-        <f t="shared" ref="AS431:AU431" si="953">AS415</f>
+        <f t="shared" ref="AS431" si="951">AS415</f>
         <v>0.46</v>
       </c>
       <c r="AT431" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU431" s="138">
         <v>0.24</v>
       </c>
       <c r="AV431" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW431" s="38">
@@ -85079,31 +85065,30 @@
         <v>114</v>
       </c>
       <c r="BF431" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG431" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH431" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI431" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ431" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ431" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK431" s="138" t="str">
-        <f t="shared" ref="BK431:BL431" si="954">BK415</f>
+        <f t="shared" ref="BK431:BL431" si="952">BK415</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL431" s="138" t="str">
-        <f t="shared" si="954"/>
+        <f t="shared" si="952"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM431" s="2" t="s">
@@ -85146,23 +85131,23 @@
         <v>274</v>
       </c>
       <c r="BZ431" s="124" t="str">
-        <f t="shared" ref="BZ431:CD431" si="955">BZ430</f>
+        <f t="shared" ref="BZ431:CD431" si="953">BZ430</f>
         <v>not compact</v>
       </c>
       <c r="CA431" s="69" t="str">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>not compact</v>
       </c>
       <c r="CB431" s="35" t="str">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC431" s="35" t="str">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>Standard</v>
       </c>
       <c r="CD431" s="40">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>-1</v>
       </c>
       <c r="CE431" s="40">
@@ -85192,11 +85177,11 @@
         <v>5</v>
       </c>
       <c r="D432" s="35">
-        <f t="shared" ref="D432:E432" si="956">D431</f>
+        <f t="shared" ref="D432:E432" si="954">D431</f>
         <v>2025</v>
       </c>
       <c r="E432" s="40" t="str">
-        <f t="shared" si="956"/>
+        <f t="shared" si="954"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F432" s="2">
@@ -85242,7 +85227,7 @@
         <v>0.62</v>
       </c>
       <c r="T432" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U432" s="38">
@@ -85264,22 +85249,22 @@
         <v>15</v>
       </c>
       <c r="AA432" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB432" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC432" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD432" s="120">
-        <f t="shared" ref="AD432:AE432" si="957">AD416</f>
+        <f t="shared" ref="AD432:AE432" si="955">AD416</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE432" s="120">
-        <f t="shared" si="957"/>
+        <f t="shared" si="955"/>
         <v>0.65</v>
       </c>
       <c r="AF432" s="2">
@@ -85310,33 +85295,33 @@
         <v>5016</v>
       </c>
       <c r="AO432" s="40">
-        <f t="shared" ref="AO432:AP432" si="958">AO431</f>
+        <f t="shared" ref="AO432:AP432" si="956">AO431</f>
         <v>0.7</v>
       </c>
       <c r="AP432" s="40" t="str">
-        <f t="shared" si="958"/>
+        <f t="shared" si="956"/>
         <v>Yes</v>
       </c>
       <c r="AQ432" s="138">
-        <f t="shared" ref="AQ432:AS432" si="959">AQ416</f>
+        <f t="shared" ref="AQ432" si="957">AQ416</f>
         <v>0.41</v>
       </c>
       <c r="AR432" s="138">
         <v>0.26</v>
       </c>
       <c r="AS432" s="138">
-        <f t="shared" ref="AS432:AU432" si="960">AS416</f>
+        <f t="shared" ref="AS432" si="958">AS416</f>
         <v>0.46</v>
       </c>
       <c r="AT432" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU432" s="138">
         <v>0.24</v>
       </c>
       <c r="AV432" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW432" s="38">
@@ -85367,31 +85352,30 @@
         <v>114</v>
       </c>
       <c r="BF432" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG432" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH432" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI432" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ432" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ432" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK432" s="138" t="str">
-        <f t="shared" ref="BK432:BL432" si="961">BK416</f>
+        <f t="shared" ref="BK432:BL432" si="959">BK416</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL432" s="138" t="str">
-        <f t="shared" si="961"/>
+        <f t="shared" si="959"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM432" s="2" t="s">
@@ -85434,23 +85418,23 @@
         <v>273</v>
       </c>
       <c r="BZ432" s="124" t="str">
-        <f t="shared" ref="BZ432:CD432" si="962">BZ431</f>
+        <f t="shared" ref="BZ432:CD432" si="960">BZ431</f>
         <v>not compact</v>
       </c>
       <c r="CA432" s="69" t="str">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>not compact</v>
       </c>
       <c r="CB432" s="35" t="str">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC432" s="35" t="str">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>Standard</v>
       </c>
       <c r="CD432" s="40">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>-1</v>
       </c>
       <c r="CE432" s="40">
@@ -85480,11 +85464,11 @@
         <v>6</v>
       </c>
       <c r="D433" s="35">
-        <f t="shared" ref="D433:E433" si="963">D432</f>
+        <f t="shared" ref="D433:E433" si="961">D432</f>
         <v>2025</v>
       </c>
       <c r="E433" s="40" t="str">
-        <f t="shared" si="963"/>
+        <f t="shared" si="961"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F433" s="2">
@@ -85530,7 +85514,7 @@
         <v>0.62</v>
       </c>
       <c r="T433" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U433" s="38">
@@ -85552,22 +85536,22 @@
         <v>15</v>
       </c>
       <c r="AA433" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB433" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AC433" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AD433" s="2">
-        <f t="shared" ref="AD433:AE433" si="964">AD417</f>
+        <f t="shared" ref="AD433:AE433" si="962">AD417</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE433" s="2">
-        <f t="shared" si="964"/>
+        <f t="shared" si="962"/>
         <v>0.69</v>
       </c>
       <c r="AF433" s="2">
@@ -85598,33 +85582,33 @@
         <v>5016</v>
       </c>
       <c r="AO433" s="40">
-        <f t="shared" ref="AO433:AP433" si="965">AO432</f>
+        <f t="shared" ref="AO433:AP433" si="963">AO432</f>
         <v>0.7</v>
       </c>
       <c r="AP433" s="40" t="str">
-        <f t="shared" si="965"/>
+        <f t="shared" si="963"/>
         <v>Yes</v>
       </c>
       <c r="AQ433" s="138">
-        <f t="shared" ref="AQ433:AS433" si="966">AQ417</f>
+        <f t="shared" ref="AQ433" si="964">AQ417</f>
         <v>0.41</v>
       </c>
       <c r="AR433" s="138">
         <v>0.26</v>
       </c>
       <c r="AS433" s="138">
-        <f t="shared" ref="AS433:AU433" si="967">AS417</f>
+        <f t="shared" ref="AS433" si="965">AS417</f>
         <v>0.46</v>
       </c>
       <c r="AT433" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU433" s="138">
         <v>0.24</v>
       </c>
       <c r="AV433" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW433" s="38">
@@ -85655,30 +85639,30 @@
         <v>114</v>
       </c>
       <c r="BF433" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG433" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH433" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BI433" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BJ433" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK433" s="138" t="str">
-        <f t="shared" ref="BK433:BL433" si="968">BK417</f>
+        <f t="shared" ref="BK433:BL433" si="966">BK417</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL433" s="138" t="str">
-        <f t="shared" si="968"/>
+        <f t="shared" si="966"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM433" s="2" t="s">
@@ -85721,23 +85705,23 @@
         <v>274</v>
       </c>
       <c r="BZ433" s="124" t="str">
-        <f t="shared" ref="BZ433:CD433" si="969">BZ432</f>
+        <f t="shared" ref="BZ433:CD433" si="967">BZ432</f>
         <v>not compact</v>
       </c>
       <c r="CA433" s="69" t="str">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>not compact</v>
       </c>
       <c r="CB433" s="35" t="str">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC433" s="35" t="str">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>Standard</v>
       </c>
       <c r="CD433" s="40">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>-1</v>
       </c>
       <c r="CE433" s="40">
@@ -85767,11 +85751,11 @@
         <v>7</v>
       </c>
       <c r="D434" s="35">
-        <f t="shared" ref="D434:E434" si="970">D433</f>
+        <f t="shared" ref="D434:E434" si="968">D433</f>
         <v>2025</v>
       </c>
       <c r="E434" s="40" t="str">
-        <f t="shared" si="970"/>
+        <f t="shared" si="968"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F434" s="2">
@@ -85817,7 +85801,7 @@
         <v>0.62</v>
       </c>
       <c r="T434" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U434" s="38">
@@ -85839,22 +85823,22 @@
         <v>15</v>
       </c>
       <c r="AA434" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB434" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AC434" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AD434" s="2">
-        <f t="shared" ref="AD434:AE434" si="971">AD418</f>
+        <f t="shared" ref="AD434:AE434" si="969">AD418</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE434" s="2">
-        <f t="shared" si="971"/>
+        <f t="shared" si="969"/>
         <v>0.69</v>
       </c>
       <c r="AF434" s="2">
@@ -85885,32 +85869,32 @@
         <v>5016</v>
       </c>
       <c r="AO434" s="40">
-        <f t="shared" ref="AO434:AP434" si="972">AO433</f>
+        <f t="shared" ref="AO434" si="970">AO433</f>
         <v>0.7</v>
       </c>
       <c r="AP434" s="121" t="s">
         <v>292</v>
       </c>
       <c r="AQ434" s="138">
-        <f t="shared" ref="AQ434:AS434" si="973">AQ418</f>
+        <f t="shared" ref="AQ434" si="971">AQ418</f>
         <v>0.41</v>
       </c>
       <c r="AR434" s="138">
         <v>0.26</v>
       </c>
       <c r="AS434" s="138">
-        <f t="shared" ref="AS434:AU434" si="974">AS418</f>
+        <f t="shared" ref="AS434" si="972">AS418</f>
         <v>0.46</v>
       </c>
       <c r="AT434" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU434" s="138">
         <v>0.24</v>
       </c>
       <c r="AV434" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW434" s="38">
@@ -85941,30 +85925,30 @@
         <v>114</v>
       </c>
       <c r="BF434" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG434" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH434" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BI434" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BJ434" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK434" s="138" t="str">
-        <f t="shared" ref="BK434:BL434" si="975">BK418</f>
+        <f t="shared" ref="BK434:BL434" si="973">BK418</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL434" s="138" t="str">
-        <f t="shared" si="975"/>
+        <f t="shared" si="973"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM434" s="2" t="s">
@@ -86007,23 +85991,23 @@
         <v>274</v>
       </c>
       <c r="BZ434" s="124" t="str">
-        <f t="shared" ref="BZ434:CD434" si="976">BZ433</f>
+        <f t="shared" ref="BZ434:CD434" si="974">BZ433</f>
         <v>not compact</v>
       </c>
       <c r="CA434" s="69" t="str">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>not compact</v>
       </c>
       <c r="CB434" s="35" t="str">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC434" s="35" t="str">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>Standard</v>
       </c>
       <c r="CD434" s="40">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>-1</v>
       </c>
       <c r="CE434" s="40">
@@ -86053,11 +86037,11 @@
         <v>8</v>
       </c>
       <c r="D435" s="35">
-        <f t="shared" ref="D435:E435" si="977">D434</f>
+        <f t="shared" ref="D435:E435" si="975">D434</f>
         <v>2025</v>
       </c>
       <c r="E435" s="40" t="str">
-        <f t="shared" si="977"/>
+        <f t="shared" si="975"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F435" s="2">
@@ -86103,7 +86087,7 @@
         <v>0.62</v>
       </c>
       <c r="T435" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U435" s="38">
@@ -86125,22 +86109,22 @@
         <v>15</v>
       </c>
       <c r="AA435" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB435" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC435" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD435" s="120">
-        <f t="shared" ref="AD435:AE435" si="978">AD419</f>
+        <f t="shared" ref="AD435:AE435" si="976">AD419</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE435" s="120">
-        <f t="shared" si="978"/>
+        <f t="shared" si="976"/>
         <v>0.69</v>
       </c>
       <c r="AF435" s="2">
@@ -86171,32 +86155,32 @@
         <v>5016</v>
       </c>
       <c r="AO435" s="40">
-        <f t="shared" ref="AO435:AP435" si="979">AO434</f>
+        <f t="shared" ref="AO435" si="977">AO434</f>
         <v>0.7</v>
       </c>
       <c r="AP435" s="38" t="s">
         <v>291</v>
       </c>
       <c r="AQ435" s="138">
-        <f t="shared" ref="AQ435:AS435" si="980">AQ419</f>
+        <f t="shared" ref="AQ435" si="978">AQ419</f>
         <v>0.41</v>
       </c>
       <c r="AR435" s="138">
         <v>0.26</v>
       </c>
       <c r="AS435" s="138">
-        <f t="shared" ref="AS435:AU435" si="981">AS419</f>
+        <f t="shared" ref="AS435" si="979">AS419</f>
         <v>0.46</v>
       </c>
       <c r="AT435" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU435" s="138">
         <v>0.24</v>
       </c>
       <c r="AV435" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW435" s="38">
@@ -86227,30 +86211,30 @@
         <v>114</v>
       </c>
       <c r="BF435" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG435" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH435" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI435" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BJ435" s="2" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="BK435" s="138" t="str">
-        <f t="shared" ref="BK435:BL435" si="982">BK419</f>
+        <f t="shared" ref="BK435:BL435" si="980">BK419</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL435" s="138" t="str">
-        <f t="shared" si="982"/>
+        <f t="shared" si="980"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM435" s="2" t="s">
@@ -86293,23 +86277,23 @@
         <v>274</v>
       </c>
       <c r="BZ435" s="124" t="str">
-        <f t="shared" ref="BZ435:CD435" si="983">BZ434</f>
+        <f t="shared" ref="BZ435:CD435" si="981">BZ434</f>
         <v>not compact</v>
       </c>
       <c r="CA435" s="69" t="str">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>not compact</v>
       </c>
       <c r="CB435" s="35" t="str">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC435" s="35" t="str">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>Standard</v>
       </c>
       <c r="CD435" s="40">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>-1</v>
       </c>
       <c r="CE435" s="40">
@@ -86339,11 +86323,11 @@
         <v>9</v>
       </c>
       <c r="D436" s="35">
-        <f t="shared" ref="D436:E436" si="984">D435</f>
+        <f t="shared" ref="D436:E436" si="982">D435</f>
         <v>2025</v>
       </c>
       <c r="E436" s="40" t="str">
-        <f t="shared" si="984"/>
+        <f t="shared" si="982"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F436" s="2">
@@ -86389,7 +86373,7 @@
         <v>0.62</v>
       </c>
       <c r="T436" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U436" s="38">
@@ -86411,22 +86395,22 @@
         <v>15</v>
       </c>
       <c r="AA436" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB436" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC436" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD436" s="120">
-        <f t="shared" ref="AD436:AE436" si="985">AD420</f>
+        <f t="shared" ref="AD436:AE436" si="983">AD420</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE436" s="120">
-        <f t="shared" si="985"/>
+        <f t="shared" si="983"/>
         <v>0.69</v>
       </c>
       <c r="AF436" s="2">
@@ -86457,33 +86441,33 @@
         <v>5016</v>
       </c>
       <c r="AO436" s="40">
-        <f t="shared" ref="AO436:AP436" si="986">AO435</f>
+        <f t="shared" ref="AO436:AP436" si="984">AO435</f>
         <v>0.7</v>
       </c>
       <c r="AP436" s="40" t="str">
-        <f t="shared" si="986"/>
+        <f t="shared" si="984"/>
         <v>Yes</v>
       </c>
       <c r="AQ436" s="138">
-        <f t="shared" ref="AQ436:AS436" si="987">AQ420</f>
+        <f t="shared" ref="AQ436" si="985">AQ420</f>
         <v>0.41</v>
       </c>
       <c r="AR436" s="138">
         <v>0.26</v>
       </c>
       <c r="AS436" s="138">
-        <f t="shared" ref="AS436:AU436" si="988">AS420</f>
+        <f t="shared" ref="AS436" si="986">AS420</f>
         <v>0.46</v>
       </c>
       <c r="AT436" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU436" s="138">
         <v>0.24</v>
       </c>
       <c r="AV436" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW436" s="38">
@@ -86514,31 +86498,30 @@
         <v>114</v>
       </c>
       <c r="BF436" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG436" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH436" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI436" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ436" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ436" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK436" s="138" t="str">
-        <f t="shared" ref="BK436:BL436" si="989">BK420</f>
+        <f t="shared" ref="BK436:BL436" si="987">BK420</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL436" s="138" t="str">
-        <f t="shared" si="989"/>
+        <f t="shared" si="987"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM436" s="2" t="s">
@@ -86581,23 +86564,23 @@
         <v>274</v>
       </c>
       <c r="BZ436" s="124" t="str">
-        <f t="shared" ref="BZ436:CD436" si="990">BZ435</f>
+        <f t="shared" ref="BZ436:CD436" si="988">BZ435</f>
         <v>not compact</v>
       </c>
       <c r="CA436" s="69" t="str">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>not compact</v>
       </c>
       <c r="CB436" s="35" t="str">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC436" s="35" t="str">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>Standard</v>
       </c>
       <c r="CD436" s="40">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>-1</v>
       </c>
       <c r="CE436" s="40">
@@ -86627,11 +86610,11 @@
         <v>10</v>
       </c>
       <c r="D437" s="35">
-        <f t="shared" ref="D437:E437" si="991">D436</f>
+        <f t="shared" ref="D437:E437" si="989">D436</f>
         <v>2025</v>
       </c>
       <c r="E437" s="40" t="str">
-        <f t="shared" si="991"/>
+        <f t="shared" si="989"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F437" s="2">
@@ -86677,7 +86660,7 @@
         <v>0.62</v>
       </c>
       <c r="T437" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U437" s="38">
@@ -86699,22 +86682,22 @@
         <v>15</v>
       </c>
       <c r="AA437" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB437" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC437" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD437" s="120">
-        <f t="shared" ref="AD437:AE437" si="992">AD421</f>
+        <f t="shared" ref="AD437:AE437" si="990">AD421</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE437" s="120">
-        <f t="shared" si="992"/>
+        <f t="shared" si="990"/>
         <v>0.65</v>
       </c>
       <c r="AF437" s="2">
@@ -86745,33 +86728,33 @@
         <v>5016</v>
       </c>
       <c r="AO437" s="40">
-        <f t="shared" ref="AO437:AP437" si="993">AO436</f>
+        <f t="shared" ref="AO437:AP437" si="991">AO436</f>
         <v>0.7</v>
       </c>
       <c r="AP437" s="40" t="str">
-        <f t="shared" si="993"/>
+        <f t="shared" si="991"/>
         <v>Yes</v>
       </c>
       <c r="AQ437" s="138">
-        <f t="shared" ref="AQ437:AS437" si="994">AQ421</f>
+        <f t="shared" ref="AQ437" si="992">AQ421</f>
         <v>0.41</v>
       </c>
       <c r="AR437" s="138">
         <v>0.26</v>
       </c>
       <c r="AS437" s="138">
-        <f t="shared" ref="AS437:AU437" si="995">AS421</f>
+        <f t="shared" ref="AS437" si="993">AS421</f>
         <v>0.46</v>
       </c>
       <c r="AT437" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU437" s="138">
         <v>0.24</v>
       </c>
       <c r="AV437" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW437" s="38">
@@ -86802,31 +86785,30 @@
         <v>114</v>
       </c>
       <c r="BF437" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG437" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH437" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI437" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ437" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ437" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK437" s="138" t="str">
-        <f t="shared" ref="BK437:BL437" si="996">BK421</f>
+        <f t="shared" ref="BK437:BL437" si="994">BK421</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL437" s="138" t="str">
-        <f t="shared" si="996"/>
+        <f t="shared" si="994"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM437" s="2" t="s">
@@ -86869,23 +86851,23 @@
         <v>274</v>
       </c>
       <c r="BZ437" s="124" t="str">
-        <f t="shared" ref="BZ437:CD437" si="997">BZ436</f>
+        <f t="shared" ref="BZ437:CD437" si="995">BZ436</f>
         <v>not compact</v>
       </c>
       <c r="CA437" s="69" t="str">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>not compact</v>
       </c>
       <c r="CB437" s="35" t="str">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC437" s="35" t="str">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>Standard</v>
       </c>
       <c r="CD437" s="40">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>-1</v>
       </c>
       <c r="CE437" s="40">
@@ -86915,11 +86897,11 @@
         <v>11</v>
       </c>
       <c r="D438" s="35">
-        <f t="shared" ref="D438:E438" si="998">D437</f>
+        <f t="shared" ref="D438:E438" si="996">D437</f>
         <v>2025</v>
       </c>
       <c r="E438" s="40" t="str">
-        <f t="shared" si="998"/>
+        <f t="shared" si="996"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F438" s="2">
@@ -86965,7 +86947,7 @@
         <v>0.62</v>
       </c>
       <c r="T438" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U438" s="38">
@@ -86987,22 +86969,22 @@
         <v>15</v>
       </c>
       <c r="AA438" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB438" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC438" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD438" s="120">
-        <f t="shared" ref="AD438:AE438" si="999">AD422</f>
+        <f t="shared" ref="AD438:AE438" si="997">AD422</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE438" s="120">
-        <f t="shared" si="999"/>
+        <f t="shared" si="997"/>
         <v>0.184</v>
       </c>
       <c r="AF438" s="2">
@@ -87033,33 +87015,33 @@
         <v>5016</v>
       </c>
       <c r="AO438" s="40">
-        <f t="shared" ref="AO438:AP438" si="1000">AO437</f>
+        <f t="shared" ref="AO438:AP438" si="998">AO437</f>
         <v>0.7</v>
       </c>
       <c r="AP438" s="40" t="str">
-        <f t="shared" si="1000"/>
+        <f t="shared" si="998"/>
         <v>Yes</v>
       </c>
       <c r="AQ438" s="138">
-        <f t="shared" ref="AQ438:AS438" si="1001">AQ422</f>
+        <f t="shared" ref="AQ438" si="999">AQ422</f>
         <v>0.41</v>
       </c>
       <c r="AR438" s="138">
         <v>0.26</v>
       </c>
       <c r="AS438" s="138">
-        <f t="shared" ref="AS438:AU438" si="1002">AS422</f>
+        <f t="shared" ref="AS438" si="1000">AS422</f>
         <v>0.46</v>
       </c>
       <c r="AT438" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU438" s="138">
         <v>0.24</v>
       </c>
       <c r="AV438" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW438" s="38">
@@ -87090,31 +87072,30 @@
         <v>114</v>
       </c>
       <c r="BF438" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG438" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH438" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI438" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ438" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ438" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK438" s="138" t="str">
-        <f t="shared" ref="BK438:BL438" si="1003">BK422</f>
+        <f t="shared" ref="BK438:BL438" si="1001">BK422</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL438" s="138" t="str">
-        <f t="shared" si="1003"/>
+        <f t="shared" si="1001"/>
         <v>T24-2022 ExtWall 8in Conc U=0.184</v>
       </c>
       <c r="BM438" s="2" t="s">
@@ -87157,23 +87138,23 @@
         <v>274</v>
       </c>
       <c r="BZ438" s="124" t="str">
-        <f t="shared" ref="BZ438:CD438" si="1004">BZ437</f>
+        <f t="shared" ref="BZ438:CD438" si="1002">BZ437</f>
         <v>not compact</v>
       </c>
       <c r="CA438" s="69" t="str">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>not compact</v>
       </c>
       <c r="CB438" s="35" t="str">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC438" s="35" t="str">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>Standard</v>
       </c>
       <c r="CD438" s="40">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>-1</v>
       </c>
       <c r="CE438" s="40">
@@ -87203,11 +87184,11 @@
         <v>12</v>
       </c>
       <c r="D439" s="35">
-        <f t="shared" ref="D439:E439" si="1005">D438</f>
+        <f t="shared" ref="D439:E439" si="1003">D438</f>
         <v>2025</v>
       </c>
       <c r="E439" s="40" t="str">
-        <f t="shared" si="1005"/>
+        <f t="shared" si="1003"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F439" s="2">
@@ -87253,7 +87234,7 @@
         <v>0.62</v>
       </c>
       <c r="T439" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U439" s="38">
@@ -87275,22 +87256,22 @@
         <v>15</v>
       </c>
       <c r="AA439" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB439" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC439" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD439" s="120">
-        <f t="shared" ref="AD439:AE439" si="1006">AD423</f>
+        <f t="shared" ref="AD439:AE439" si="1004">AD423</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE439" s="120">
-        <f t="shared" si="1006"/>
+        <f t="shared" si="1004"/>
         <v>0.253</v>
       </c>
       <c r="AF439" s="2">
@@ -87321,33 +87302,33 @@
         <v>5016</v>
       </c>
       <c r="AO439" s="40">
-        <f t="shared" ref="AO439:AP439" si="1007">AO438</f>
+        <f t="shared" ref="AO439:AP439" si="1005">AO438</f>
         <v>0.7</v>
       </c>
       <c r="AP439" s="40" t="str">
-        <f t="shared" si="1007"/>
+        <f t="shared" si="1005"/>
         <v>Yes</v>
       </c>
       <c r="AQ439" s="138">
-        <f t="shared" ref="AQ439:AS439" si="1008">AQ423</f>
+        <f t="shared" ref="AQ439" si="1006">AQ423</f>
         <v>0.41</v>
       </c>
       <c r="AR439" s="138">
         <v>0.26</v>
       </c>
       <c r="AS439" s="138">
-        <f t="shared" ref="AS439:AU439" si="1009">AS423</f>
+        <f t="shared" ref="AS439" si="1007">AS423</f>
         <v>0.46</v>
       </c>
       <c r="AT439" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU439" s="138">
         <v>0.24</v>
       </c>
       <c r="AV439" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW439" s="38">
@@ -87378,31 +87359,30 @@
         <v>114</v>
       </c>
       <c r="BF439" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG439" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH439" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI439" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ439" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ439" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK439" s="138" t="str">
-        <f t="shared" ref="BK439:BL439" si="1010">BK423</f>
+        <f t="shared" ref="BK439:BL439" si="1008">BK423</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL439" s="138" t="str">
-        <f t="shared" si="1010"/>
+        <f t="shared" si="1008"/>
         <v>T24-2022 ExtWall 8in Conc U=0.253</v>
       </c>
       <c r="BM439" s="2" t="s">
@@ -87445,23 +87425,23 @@
         <v>274</v>
       </c>
       <c r="BZ439" s="124" t="str">
-        <f t="shared" ref="BZ439:CD439" si="1011">BZ438</f>
+        <f t="shared" ref="BZ439:CD439" si="1009">BZ438</f>
         <v>not compact</v>
       </c>
       <c r="CA439" s="69" t="str">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>not compact</v>
       </c>
       <c r="CB439" s="35" t="str">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC439" s="35" t="str">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>Standard</v>
       </c>
       <c r="CD439" s="40">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>-1</v>
       </c>
       <c r="CE439" s="40">
@@ -87491,11 +87471,11 @@
         <v>13</v>
       </c>
       <c r="D440" s="35">
-        <f t="shared" ref="D440:E440" si="1012">D439</f>
+        <f t="shared" ref="D440:E440" si="1010">D439</f>
         <v>2025</v>
       </c>
       <c r="E440" s="40" t="str">
-        <f t="shared" si="1012"/>
+        <f t="shared" si="1010"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F440" s="2">
@@ -87541,7 +87521,7 @@
         <v>0.62</v>
       </c>
       <c r="T440" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U440" s="38">
@@ -87563,22 +87543,22 @@
         <v>15</v>
       </c>
       <c r="AA440" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB440" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC440" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD440" s="120">
-        <f t="shared" ref="AD440:AE440" si="1013">AD424</f>
+        <f t="shared" ref="AD440:AE440" si="1011">AD424</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE440" s="120">
-        <f t="shared" si="1013"/>
+        <f t="shared" si="1011"/>
         <v>0.21099999999999999</v>
       </c>
       <c r="AF440" s="2">
@@ -87609,33 +87589,33 @@
         <v>5016</v>
       </c>
       <c r="AO440" s="40">
-        <f t="shared" ref="AO440:AP440" si="1014">AO439</f>
+        <f t="shared" ref="AO440:AP440" si="1012">AO439</f>
         <v>0.7</v>
       </c>
       <c r="AP440" s="40" t="str">
-        <f t="shared" si="1014"/>
+        <f t="shared" si="1012"/>
         <v>Yes</v>
       </c>
       <c r="AQ440" s="138">
-        <f t="shared" ref="AQ440:AS440" si="1015">AQ424</f>
+        <f t="shared" ref="AQ440" si="1013">AQ424</f>
         <v>0.41</v>
       </c>
       <c r="AR440" s="138">
         <v>0.26</v>
       </c>
       <c r="AS440" s="138">
-        <f t="shared" ref="AS440:AU440" si="1016">AS424</f>
+        <f t="shared" ref="AS440" si="1014">AS424</f>
         <v>0.46</v>
       </c>
       <c r="AT440" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU440" s="138">
         <v>0.24</v>
       </c>
       <c r="AV440" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW440" s="38">
@@ -87666,31 +87646,30 @@
         <v>114</v>
       </c>
       <c r="BF440" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG440" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH440" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI440" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ440" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ440" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK440" s="138" t="str">
-        <f t="shared" ref="BK440:BL440" si="1017">BK424</f>
+        <f t="shared" ref="BK440:BL440" si="1015">BK424</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL440" s="138" t="str">
-        <f t="shared" si="1017"/>
+        <f t="shared" si="1015"/>
         <v>T24-2022 ExtWall 8in Conc U=0.211</v>
       </c>
       <c r="BM440" s="2" t="s">
@@ -87733,23 +87712,23 @@
         <v>274</v>
       </c>
       <c r="BZ440" s="124" t="str">
-        <f t="shared" ref="BZ440:CD440" si="1018">BZ439</f>
+        <f t="shared" ref="BZ440:CD440" si="1016">BZ439</f>
         <v>not compact</v>
       </c>
       <c r="CA440" s="69" t="str">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>not compact</v>
       </c>
       <c r="CB440" s="35" t="str">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC440" s="35" t="str">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>Standard</v>
       </c>
       <c r="CD440" s="40">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>-1</v>
       </c>
       <c r="CE440" s="40">
@@ -87779,11 +87758,11 @@
         <v>14</v>
       </c>
       <c r="D441" s="35">
-        <f t="shared" ref="D441:E441" si="1019">D440</f>
+        <f t="shared" ref="D441:E441" si="1017">D440</f>
         <v>2025</v>
       </c>
       <c r="E441" s="40" t="str">
-        <f t="shared" si="1019"/>
+        <f t="shared" si="1017"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F441" s="2">
@@ -87829,7 +87808,7 @@
         <v>0.62</v>
       </c>
       <c r="T441" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U441" s="38">
@@ -87851,22 +87830,22 @@
         <v>15</v>
       </c>
       <c r="AA441" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB441" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC441" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD441" s="120">
-        <f t="shared" ref="AD441:AE441" si="1020">AD425</f>
+        <f t="shared" ref="AD441:AE441" si="1018">AD425</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE441" s="120">
-        <f t="shared" si="1020"/>
+        <f t="shared" si="1018"/>
         <v>0.184</v>
       </c>
       <c r="AF441" s="2">
@@ -87897,33 +87876,33 @@
         <v>5016</v>
       </c>
       <c r="AO441" s="40">
-        <f t="shared" ref="AO441:AP441" si="1021">AO440</f>
+        <f t="shared" ref="AO441:AP441" si="1019">AO440</f>
         <v>0.7</v>
       </c>
       <c r="AP441" s="40" t="str">
-        <f t="shared" si="1021"/>
+        <f t="shared" si="1019"/>
         <v>Yes</v>
       </c>
       <c r="AQ441" s="138">
-        <f t="shared" ref="AQ441:AS441" si="1022">AQ425</f>
+        <f t="shared" ref="AQ441" si="1020">AQ425</f>
         <v>0.41</v>
       </c>
       <c r="AR441" s="138">
         <v>0.25</v>
       </c>
       <c r="AS441" s="138">
-        <f t="shared" ref="AS441:AU441" si="1023">AS425</f>
+        <f t="shared" ref="AS441" si="1021">AS425</f>
         <v>0.46</v>
       </c>
       <c r="AT441" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU441" s="138">
         <v>0.24</v>
       </c>
       <c r="AV441" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW441" s="38">
@@ -87954,31 +87933,30 @@
         <v>114</v>
       </c>
       <c r="BF441" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG441" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH441" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI441" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ441" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ441" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK441" s="138" t="str">
-        <f t="shared" ref="BK441:BL441" si="1024">BK425</f>
+        <f t="shared" ref="BK441:BL441" si="1022">BK425</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL441" s="138" t="str">
-        <f t="shared" si="1024"/>
+        <f t="shared" si="1022"/>
         <v>T24-2022 ExtWall 8in Conc U=0.184</v>
       </c>
       <c r="BM441" s="2" t="s">
@@ -88021,23 +87999,23 @@
         <v>274</v>
       </c>
       <c r="BZ441" s="124" t="str">
-        <f t="shared" ref="BZ441:CD441" si="1025">BZ440</f>
+        <f t="shared" ref="BZ441:CD441" si="1023">BZ440</f>
         <v>not compact</v>
       </c>
       <c r="CA441" s="69" t="str">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>not compact</v>
       </c>
       <c r="CB441" s="35" t="str">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC441" s="35" t="str">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>Standard</v>
       </c>
       <c r="CD441" s="40">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>-1</v>
       </c>
       <c r="CE441" s="40">
@@ -88067,11 +88045,11 @@
         <v>15</v>
       </c>
       <c r="D442" s="35">
-        <f t="shared" ref="D442:E442" si="1026">D441</f>
+        <f t="shared" ref="D442:E442" si="1024">D441</f>
         <v>2025</v>
       </c>
       <c r="E442" s="40" t="str">
-        <f t="shared" si="1026"/>
+        <f t="shared" si="1024"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F442" s="2">
@@ -88117,7 +88095,7 @@
         <v>0.62</v>
       </c>
       <c r="T442" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U442" s="38">
@@ -88139,22 +88117,22 @@
         <v>15</v>
       </c>
       <c r="AA442" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB442" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC442" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD442" s="120">
-        <f t="shared" ref="AD442:AE442" si="1027">AD426</f>
+        <f t="shared" ref="AD442:AE442" si="1025">AD426</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE442" s="120">
-        <f t="shared" si="1027"/>
+        <f t="shared" si="1025"/>
         <v>0.184</v>
       </c>
       <c r="AF442" s="2">
@@ -88185,33 +88163,33 @@
         <v>5016</v>
       </c>
       <c r="AO442" s="40">
-        <f t="shared" ref="AO442:AP442" si="1028">AO441</f>
+        <f t="shared" ref="AO442:AP442" si="1026">AO441</f>
         <v>0.7</v>
       </c>
       <c r="AP442" s="40" t="str">
-        <f t="shared" si="1028"/>
+        <f t="shared" si="1026"/>
         <v>Yes</v>
       </c>
       <c r="AQ442" s="138">
-        <f t="shared" ref="AQ442:AS442" si="1029">AQ426</f>
+        <f t="shared" ref="AQ442" si="1027">AQ426</f>
         <v>0.41</v>
       </c>
       <c r="AR442" s="138">
         <v>0.26</v>
       </c>
       <c r="AS442" s="138">
-        <f t="shared" ref="AS442:AU442" si="1030">AS426</f>
+        <f t="shared" ref="AS442" si="1028">AS426</f>
         <v>0.46</v>
       </c>
       <c r="AT442" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU442" s="138">
         <v>0.24</v>
       </c>
       <c r="AV442" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW442" s="38">
@@ -88242,31 +88220,30 @@
         <v>114</v>
       </c>
       <c r="BF442" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG442" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH442" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI442" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ442" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ442" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK442" s="138" t="str">
-        <f t="shared" ref="BK442:BL442" si="1031">BK426</f>
+        <f t="shared" ref="BK442:BL442" si="1029">BK426</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL442" s="138" t="str">
-        <f t="shared" si="1031"/>
+        <f t="shared" si="1029"/>
         <v>T24-2022 ExtWall 8in Conc U=0.184</v>
       </c>
       <c r="BM442" s="2" t="s">
@@ -88309,23 +88286,23 @@
         <v>274</v>
       </c>
       <c r="BZ442" s="124" t="str">
-        <f t="shared" ref="BZ442:CD442" si="1032">BZ441</f>
+        <f t="shared" ref="BZ442:CD442" si="1030">BZ441</f>
         <v>not compact</v>
       </c>
       <c r="CA442" s="69" t="str">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>not compact</v>
       </c>
       <c r="CB442" s="35" t="str">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC442" s="35" t="str">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>Standard</v>
       </c>
       <c r="CD442" s="40">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>-1</v>
       </c>
       <c r="CE442" s="40">
@@ -88355,11 +88332,11 @@
         <v>16</v>
       </c>
       <c r="D443" s="35">
-        <f t="shared" ref="D443:E443" si="1033">D442</f>
+        <f t="shared" ref="D443:E443" si="1031">D442</f>
         <v>2025</v>
       </c>
       <c r="E443" s="40" t="str">
-        <f t="shared" si="1033"/>
+        <f t="shared" si="1031"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F443" s="2">
@@ -88405,7 +88382,7 @@
         <v>0.62</v>
       </c>
       <c r="T443" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U443" s="38">
@@ -88427,22 +88404,22 @@
         <v>15</v>
       </c>
       <c r="AA443" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB443" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC443" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD443" s="120">
-        <f t="shared" ref="AD443:AE443" si="1034">AD427</f>
+        <f t="shared" ref="AD443:AE443" si="1032">AD427</f>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AE443" s="120">
-        <f t="shared" si="1034"/>
+        <f t="shared" si="1032"/>
         <v>0.16</v>
       </c>
       <c r="AF443" s="2">
@@ -88473,33 +88450,33 @@
         <v>10016</v>
       </c>
       <c r="AO443" s="40">
-        <f t="shared" ref="AO443:AP443" si="1035">AO442</f>
+        <f t="shared" ref="AO443:AP443" si="1033">AO442</f>
         <v>0.7</v>
       </c>
       <c r="AP443" s="40" t="str">
-        <f t="shared" si="1035"/>
+        <f t="shared" si="1033"/>
         <v>Yes</v>
       </c>
       <c r="AQ443" s="138">
-        <f t="shared" ref="AQ443:AS443" si="1036">AQ427</f>
+        <f t="shared" ref="AQ443" si="1034">AQ427</f>
         <v>0.38</v>
       </c>
       <c r="AR443" s="138">
         <v>0.25</v>
       </c>
       <c r="AS443" s="138">
-        <f t="shared" ref="AS443:AU443" si="1037">AS427</f>
+        <f t="shared" ref="AS443" si="1035">AS427</f>
         <v>0.46</v>
       </c>
       <c r="AT443" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.38</v>
       </c>
       <c r="AU443" s="138">
         <v>0.24</v>
       </c>
       <c r="AV443" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW443" s="38">
@@ -88530,31 +88507,30 @@
         <v>114</v>
       </c>
       <c r="BF443" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG443" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH443" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI443" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ443" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ443" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK443" s="138" t="str">
-        <f t="shared" ref="BK443:BL443" si="1038">BK427</f>
+        <f t="shared" ref="BK443:BL443" si="1036">BK427</f>
         <v>T24-2022 ExtWall 6in Conc R17</v>
       </c>
       <c r="BL443" s="138" t="str">
-        <f t="shared" si="1038"/>
+        <f t="shared" si="1036"/>
         <v>T24-2022 ExtWall 10in Conc U=0.160</v>
       </c>
       <c r="BM443" s="2" t="s">
@@ -88597,23 +88573,23 @@
         <v>274</v>
       </c>
       <c r="BZ443" s="124" t="str">
-        <f t="shared" ref="BZ443:CD443" si="1039">BZ442</f>
+        <f t="shared" ref="BZ443:CD443" si="1037">BZ442</f>
         <v>not compact</v>
       </c>
       <c r="CA443" s="69" t="str">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>not compact</v>
       </c>
       <c r="CB443" s="35" t="str">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC443" s="35" t="str">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>Standard</v>
       </c>
       <c r="CD443" s="40">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>-1</v>
       </c>
       <c r="CE443" s="121">

</xml_diff>

<commit_message>
SVN Revision #8146 by jireh360       Ticket #3455 MF Indirectly Conditioned Zones
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/shared/T24RClimateZoneCodeBaselines.xlsx
+++ b/RulesetDev/Rulesets/shared/T24RClimateZoneCodeBaselines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\360 Local\_CBECC Com MFamIndirectCondZn\RulesetDev\Rulesets\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51803EDA-A723-4BFF-B15B-8A70BC2FD5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFA1269-2898-45AA-9024-B16909BE4ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2715" windowWidth="25800" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="47565" windowHeight="19425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T24RClimateZoneCodeBaselines" sheetId="1" r:id="rId1"/>
@@ -2579,7 +2579,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9371" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9395" uniqueCount="398">
   <si>
     <t>;</t>
   </si>
@@ -5185,8 +5185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FM444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D429" sqref="D429"/>
+    <sheetView tabSelected="1" topLeftCell="AW391" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BJ420" sqref="BJ420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -79843,7 +79843,7 @@
         <v>374</v>
       </c>
       <c r="BJ412" s="2" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="BK412" s="2" t="s">
         <v>376</v>
@@ -80111,9 +80111,8 @@
       <c r="BI413" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ413" s="35" t="str">
-        <f>BJ412</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ413" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK413" s="2" t="s">
         <v>376</v>
@@ -80386,9 +80385,8 @@
       <c r="BI414" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ414" s="35" t="str">
-        <f t="shared" ref="BJ414:BJ427" si="890">BJ413</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ414" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK414" s="2" t="s">
         <v>376</v>
@@ -80436,23 +80434,23 @@
         <v>273</v>
       </c>
       <c r="BZ414" s="124" t="str">
-        <f t="shared" ref="BZ414:CD414" si="891">BZ413</f>
+        <f t="shared" ref="BZ414:CD414" si="890">BZ413</f>
         <v>not compact</v>
       </c>
       <c r="CA414" s="69" t="str">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>not compact</v>
       </c>
       <c r="CB414" s="35" t="str">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC414" s="35" t="str">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>Standard</v>
       </c>
       <c r="CD414" s="40">
-        <f t="shared" si="891"/>
+        <f t="shared" si="890"/>
         <v>-1</v>
       </c>
       <c r="CE414" s="40">
@@ -80482,11 +80480,11 @@
         <v>4</v>
       </c>
       <c r="D415" s="35">
-        <f t="shared" ref="D415:E415" si="892">D414</f>
+        <f t="shared" ref="D415:E415" si="891">D414</f>
         <v>2025</v>
       </c>
       <c r="E415" s="40" t="str">
-        <f t="shared" si="892"/>
+        <f t="shared" si="891"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F415" s="2">
@@ -80596,11 +80594,11 @@
         <v>5016</v>
       </c>
       <c r="AO415" s="40">
-        <f t="shared" ref="AO415:AP415" si="893">AO414</f>
+        <f t="shared" ref="AO415:AP415" si="892">AO414</f>
         <v>0.7</v>
       </c>
       <c r="AP415" s="40" t="str">
-        <f t="shared" si="893"/>
+        <f t="shared" si="892"/>
         <v>Yes</v>
       </c>
       <c r="AQ415" s="138">
@@ -80661,9 +80659,8 @@
       <c r="BI415" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ415" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ415" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK415" s="2" t="s">
         <v>376</v>
@@ -80711,23 +80708,23 @@
         <v>274</v>
       </c>
       <c r="BZ415" s="124" t="str">
-        <f t="shared" ref="BZ415:CD415" si="894">BZ414</f>
+        <f t="shared" ref="BZ415:CD415" si="893">BZ414</f>
         <v>not compact</v>
       </c>
       <c r="CA415" s="69" t="str">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>not compact</v>
       </c>
       <c r="CB415" s="35" t="str">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC415" s="35" t="str">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>Standard</v>
       </c>
       <c r="CD415" s="40">
-        <f t="shared" si="894"/>
+        <f t="shared" si="893"/>
         <v>-1</v>
       </c>
       <c r="CE415" s="40">
@@ -80757,11 +80754,11 @@
         <v>5</v>
       </c>
       <c r="D416" s="35">
-        <f t="shared" ref="D416:E416" si="895">D415</f>
+        <f t="shared" ref="D416:E416" si="894">D415</f>
         <v>2025</v>
       </c>
       <c r="E416" s="40" t="str">
-        <f t="shared" si="895"/>
+        <f t="shared" si="894"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F416" s="2">
@@ -80871,11 +80868,11 @@
         <v>5016</v>
       </c>
       <c r="AO416" s="40">
-        <f t="shared" ref="AO416:AP416" si="896">AO415</f>
+        <f t="shared" ref="AO416:AP416" si="895">AO415</f>
         <v>0.7</v>
       </c>
       <c r="AP416" s="40" t="str">
-        <f t="shared" si="896"/>
+        <f t="shared" si="895"/>
         <v>Yes</v>
       </c>
       <c r="AQ416" s="138">
@@ -80936,9 +80933,8 @@
       <c r="BI416" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ416" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ416" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK416" s="2" t="s">
         <v>376</v>
@@ -80986,23 +80982,23 @@
         <v>273</v>
       </c>
       <c r="BZ416" s="124" t="str">
-        <f t="shared" ref="BZ416:CD416" si="897">BZ415</f>
+        <f t="shared" ref="BZ416:CD416" si="896">BZ415</f>
         <v>not compact</v>
       </c>
       <c r="CA416" s="69" t="str">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>not compact</v>
       </c>
       <c r="CB416" s="35" t="str">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC416" s="35" t="str">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>Standard</v>
       </c>
       <c r="CD416" s="40">
-        <f t="shared" si="897"/>
+        <f t="shared" si="896"/>
         <v>-1</v>
       </c>
       <c r="CE416" s="40">
@@ -81032,11 +81028,11 @@
         <v>6</v>
       </c>
       <c r="D417" s="35">
-        <f t="shared" ref="D417:E417" si="898">D416</f>
+        <f t="shared" ref="D417:E417" si="897">D416</f>
         <v>2025</v>
       </c>
       <c r="E417" s="40" t="str">
-        <f t="shared" si="898"/>
+        <f t="shared" si="897"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F417" s="2">
@@ -81146,11 +81142,11 @@
         <v>5016</v>
       </c>
       <c r="AO417" s="40">
-        <f t="shared" ref="AO417:AP419" si="899">AO416</f>
+        <f t="shared" ref="AO417:AP419" si="898">AO416</f>
         <v>0.7</v>
       </c>
       <c r="AP417" s="40" t="str">
-        <f t="shared" si="899"/>
+        <f t="shared" si="898"/>
         <v>Yes</v>
       </c>
       <c r="AQ417" s="138">
@@ -81212,7 +81208,7 @@
         <v>373</v>
       </c>
       <c r="BJ417" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK417" s="2" t="s">
         <v>376</v>
@@ -81260,23 +81256,23 @@
         <v>274</v>
       </c>
       <c r="BZ417" s="124" t="str">
-        <f t="shared" ref="BZ417:CD417" si="900">BZ416</f>
+        <f t="shared" ref="BZ417:CD417" si="899">BZ416</f>
         <v>not compact</v>
       </c>
       <c r="CA417" s="69" t="str">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>not compact</v>
       </c>
       <c r="CB417" s="35" t="str">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC417" s="35" t="str">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>Standard</v>
       </c>
       <c r="CD417" s="40">
-        <f t="shared" si="900"/>
+        <f t="shared" si="899"/>
         <v>-1</v>
       </c>
       <c r="CE417" s="40">
@@ -81306,11 +81302,11 @@
         <v>7</v>
       </c>
       <c r="D418" s="35">
-        <f t="shared" ref="D418:E418" si="901">D417</f>
+        <f t="shared" ref="D418:E418" si="900">D417</f>
         <v>2025</v>
       </c>
       <c r="E418" s="40" t="str">
-        <f t="shared" si="901"/>
+        <f t="shared" si="900"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F418" s="2">
@@ -81420,7 +81416,7 @@
         <v>5016</v>
       </c>
       <c r="AO418" s="40">
-        <f t="shared" si="899"/>
+        <f t="shared" si="898"/>
         <v>0.7</v>
       </c>
       <c r="AP418" s="121" t="s">
@@ -81485,7 +81481,7 @@
         <v>373</v>
       </c>
       <c r="BJ418" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK418" s="2" t="s">
         <v>376</v>
@@ -81533,23 +81529,23 @@
         <v>274</v>
       </c>
       <c r="BZ418" s="124" t="str">
-        <f t="shared" ref="BZ418:CD418" si="902">BZ417</f>
+        <f t="shared" ref="BZ418:CD418" si="901">BZ417</f>
         <v>not compact</v>
       </c>
       <c r="CA418" s="69" t="str">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>not compact</v>
       </c>
       <c r="CB418" s="35" t="str">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC418" s="35" t="str">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>Standard</v>
       </c>
       <c r="CD418" s="40">
-        <f t="shared" si="902"/>
+        <f t="shared" si="901"/>
         <v>-1</v>
       </c>
       <c r="CE418" s="40">
@@ -81579,11 +81575,11 @@
         <v>8</v>
       </c>
       <c r="D419" s="35">
-        <f t="shared" ref="D419:E419" si="903">D418</f>
+        <f t="shared" ref="D419:E419" si="902">D418</f>
         <v>2025</v>
       </c>
       <c r="E419" s="40" t="str">
-        <f t="shared" si="903"/>
+        <f t="shared" si="902"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F419" s="2">
@@ -81693,7 +81689,7 @@
         <v>5016</v>
       </c>
       <c r="AO419" s="40">
-        <f t="shared" si="899"/>
+        <f t="shared" si="898"/>
         <v>0.7</v>
       </c>
       <c r="AP419" s="38" t="s">
@@ -81758,7 +81754,7 @@
         <v>374</v>
       </c>
       <c r="BJ419" s="2" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="BK419" s="2" t="s">
         <v>376</v>
@@ -81806,23 +81802,23 @@
         <v>274</v>
       </c>
       <c r="BZ419" s="124" t="str">
-        <f t="shared" ref="BZ419:CD419" si="904">BZ418</f>
+        <f t="shared" ref="BZ419:CD419" si="903">BZ418</f>
         <v>not compact</v>
       </c>
       <c r="CA419" s="69" t="str">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>not compact</v>
       </c>
       <c r="CB419" s="35" t="str">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC419" s="35" t="str">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>Standard</v>
       </c>
       <c r="CD419" s="40">
-        <f t="shared" si="904"/>
+        <f t="shared" si="903"/>
         <v>-1</v>
       </c>
       <c r="CE419" s="40">
@@ -81852,11 +81848,11 @@
         <v>9</v>
       </c>
       <c r="D420" s="35">
-        <f t="shared" ref="D420:E420" si="905">D419</f>
+        <f t="shared" ref="D420:E420" si="904">D419</f>
         <v>2025</v>
       </c>
       <c r="E420" s="40" t="str">
-        <f t="shared" si="905"/>
+        <f t="shared" si="904"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F420" s="2">
@@ -81966,11 +81962,11 @@
         <v>5016</v>
       </c>
       <c r="AO420" s="40">
-        <f t="shared" ref="AO420:AP420" si="906">AO419</f>
+        <f t="shared" ref="AO420:AP420" si="905">AO419</f>
         <v>0.7</v>
       </c>
       <c r="AP420" s="40" t="str">
-        <f t="shared" si="906"/>
+        <f t="shared" si="905"/>
         <v>Yes</v>
       </c>
       <c r="AQ420" s="138">
@@ -82031,9 +82027,8 @@
       <c r="BI420" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ420" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ420" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK420" s="2" t="s">
         <v>376</v>
@@ -82081,23 +82076,23 @@
         <v>274</v>
       </c>
       <c r="BZ420" s="124" t="str">
-        <f t="shared" ref="BZ420:CD420" si="907">BZ419</f>
+        <f t="shared" ref="BZ420:CD420" si="906">BZ419</f>
         <v>not compact</v>
       </c>
       <c r="CA420" s="69" t="str">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>not compact</v>
       </c>
       <c r="CB420" s="35" t="str">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC420" s="35" t="str">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>Standard</v>
       </c>
       <c r="CD420" s="40">
-        <f t="shared" si="907"/>
+        <f t="shared" si="906"/>
         <v>-1</v>
       </c>
       <c r="CE420" s="40">
@@ -82127,11 +82122,11 @@
         <v>10</v>
       </c>
       <c r="D421" s="35">
-        <f t="shared" ref="D421:E421" si="908">D420</f>
+        <f t="shared" ref="D421:E421" si="907">D420</f>
         <v>2025</v>
       </c>
       <c r="E421" s="40" t="str">
-        <f t="shared" si="908"/>
+        <f t="shared" si="907"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F421" s="2">
@@ -82241,11 +82236,11 @@
         <v>5016</v>
       </c>
       <c r="AO421" s="40">
-        <f t="shared" ref="AO421:AP421" si="909">AO420</f>
+        <f t="shared" ref="AO421:AP421" si="908">AO420</f>
         <v>0.7</v>
       </c>
       <c r="AP421" s="40" t="str">
-        <f t="shared" si="909"/>
+        <f t="shared" si="908"/>
         <v>Yes</v>
       </c>
       <c r="AQ421" s="138">
@@ -82306,9 +82301,8 @@
       <c r="BI421" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ421" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ421" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK421" s="2" t="s">
         <v>376</v>
@@ -82356,23 +82350,23 @@
         <v>274</v>
       </c>
       <c r="BZ421" s="124" t="str">
-        <f t="shared" ref="BZ421:CD421" si="910">BZ420</f>
+        <f t="shared" ref="BZ421:CD421" si="909">BZ420</f>
         <v>not compact</v>
       </c>
       <c r="CA421" s="69" t="str">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>not compact</v>
       </c>
       <c r="CB421" s="35" t="str">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC421" s="35" t="str">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>Standard</v>
       </c>
       <c r="CD421" s="40">
-        <f t="shared" si="910"/>
+        <f t="shared" si="909"/>
         <v>-1</v>
       </c>
       <c r="CE421" s="40">
@@ -82402,11 +82396,11 @@
         <v>11</v>
       </c>
       <c r="D422" s="35">
-        <f t="shared" ref="D422:E422" si="911">D421</f>
+        <f t="shared" ref="D422:E422" si="910">D421</f>
         <v>2025</v>
       </c>
       <c r="E422" s="40" t="str">
-        <f t="shared" si="911"/>
+        <f t="shared" si="910"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F422" s="2">
@@ -82516,11 +82510,11 @@
         <v>5016</v>
       </c>
       <c r="AO422" s="40">
-        <f t="shared" ref="AO422:AP422" si="912">AO421</f>
+        <f t="shared" ref="AO422:AP422" si="911">AO421</f>
         <v>0.7</v>
       </c>
       <c r="AP422" s="40" t="str">
-        <f t="shared" si="912"/>
+        <f t="shared" si="911"/>
         <v>Yes</v>
       </c>
       <c r="AQ422" s="138">
@@ -82581,9 +82575,8 @@
       <c r="BI422" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ422" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ422" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK422" s="2" t="s">
         <v>376</v>
@@ -82631,23 +82624,23 @@
         <v>274</v>
       </c>
       <c r="BZ422" s="124" t="str">
-        <f t="shared" ref="BZ422:CD422" si="913">BZ421</f>
+        <f t="shared" ref="BZ422:CD422" si="912">BZ421</f>
         <v>not compact</v>
       </c>
       <c r="CA422" s="69" t="str">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>not compact</v>
       </c>
       <c r="CB422" s="35" t="str">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC422" s="35" t="str">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>Standard</v>
       </c>
       <c r="CD422" s="40">
-        <f t="shared" si="913"/>
+        <f t="shared" si="912"/>
         <v>-1</v>
       </c>
       <c r="CE422" s="40">
@@ -82677,11 +82670,11 @@
         <v>12</v>
       </c>
       <c r="D423" s="35">
-        <f t="shared" ref="D423:E423" si="914">D422</f>
+        <f t="shared" ref="D423:E423" si="913">D422</f>
         <v>2025</v>
       </c>
       <c r="E423" s="40" t="str">
-        <f t="shared" si="914"/>
+        <f t="shared" si="913"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F423" s="2">
@@ -82791,11 +82784,11 @@
         <v>5016</v>
       </c>
       <c r="AO423" s="40">
-        <f t="shared" ref="AO423:AP423" si="915">AO422</f>
+        <f t="shared" ref="AO423:AP423" si="914">AO422</f>
         <v>0.7</v>
       </c>
       <c r="AP423" s="40" t="str">
-        <f t="shared" si="915"/>
+        <f t="shared" si="914"/>
         <v>Yes</v>
       </c>
       <c r="AQ423" s="138">
@@ -82856,9 +82849,8 @@
       <c r="BI423" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ423" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ423" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK423" s="2" t="s">
         <v>376</v>
@@ -82906,23 +82898,23 @@
         <v>274</v>
       </c>
       <c r="BZ423" s="124" t="str">
-        <f t="shared" ref="BZ423:CD423" si="916">BZ422</f>
+        <f t="shared" ref="BZ423:CD423" si="915">BZ422</f>
         <v>not compact</v>
       </c>
       <c r="CA423" s="69" t="str">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>not compact</v>
       </c>
       <c r="CB423" s="35" t="str">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC423" s="35" t="str">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>Standard</v>
       </c>
       <c r="CD423" s="40">
-        <f t="shared" si="916"/>
+        <f t="shared" si="915"/>
         <v>-1</v>
       </c>
       <c r="CE423" s="40">
@@ -82952,11 +82944,11 @@
         <v>13</v>
       </c>
       <c r="D424" s="35">
-        <f t="shared" ref="D424:E424" si="917">D423</f>
+        <f t="shared" ref="D424:E424" si="916">D423</f>
         <v>2025</v>
       </c>
       <c r="E424" s="40" t="str">
-        <f t="shared" si="917"/>
+        <f t="shared" si="916"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F424" s="2">
@@ -83066,11 +83058,11 @@
         <v>5016</v>
       </c>
       <c r="AO424" s="40">
-        <f t="shared" ref="AO424:AP424" si="918">AO423</f>
+        <f t="shared" ref="AO424:AP424" si="917">AO423</f>
         <v>0.7</v>
       </c>
       <c r="AP424" s="40" t="str">
-        <f t="shared" si="918"/>
+        <f t="shared" si="917"/>
         <v>Yes</v>
       </c>
       <c r="AQ424" s="138">
@@ -83131,9 +83123,8 @@
       <c r="BI424" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ424" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ424" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK424" s="2" t="s">
         <v>376</v>
@@ -83181,23 +83172,23 @@
         <v>274</v>
       </c>
       <c r="BZ424" s="124" t="str">
-        <f t="shared" ref="BZ424:CD424" si="919">BZ423</f>
+        <f t="shared" ref="BZ424:CD424" si="918">BZ423</f>
         <v>not compact</v>
       </c>
       <c r="CA424" s="69" t="str">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>not compact</v>
       </c>
       <c r="CB424" s="35" t="str">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC424" s="35" t="str">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>Standard</v>
       </c>
       <c r="CD424" s="40">
-        <f t="shared" si="919"/>
+        <f t="shared" si="918"/>
         <v>-1</v>
       </c>
       <c r="CE424" s="40">
@@ -83227,11 +83218,11 @@
         <v>14</v>
       </c>
       <c r="D425" s="35">
-        <f t="shared" ref="D425:E425" si="920">D424</f>
+        <f t="shared" ref="D425:E425" si="919">D424</f>
         <v>2025</v>
       </c>
       <c r="E425" s="40" t="str">
-        <f t="shared" si="920"/>
+        <f t="shared" si="919"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F425" s="2">
@@ -83341,11 +83332,11 @@
         <v>5016</v>
       </c>
       <c r="AO425" s="40">
-        <f t="shared" ref="AO425:AP425" si="921">AO424</f>
+        <f t="shared" ref="AO425:AP425" si="920">AO424</f>
         <v>0.7</v>
       </c>
       <c r="AP425" s="40" t="str">
-        <f t="shared" si="921"/>
+        <f t="shared" si="920"/>
         <v>Yes</v>
       </c>
       <c r="AQ425" s="138">
@@ -83406,9 +83397,8 @@
       <c r="BI425" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ425" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ425" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK425" s="2" t="s">
         <v>376</v>
@@ -83456,23 +83446,23 @@
         <v>274</v>
       </c>
       <c r="BZ425" s="124" t="str">
-        <f t="shared" ref="BZ425:CD425" si="922">BZ424</f>
+        <f t="shared" ref="BZ425:CD425" si="921">BZ424</f>
         <v>not compact</v>
       </c>
       <c r="CA425" s="69" t="str">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>not compact</v>
       </c>
       <c r="CB425" s="35" t="str">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC425" s="35" t="str">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>Standard</v>
       </c>
       <c r="CD425" s="40">
-        <f t="shared" si="922"/>
+        <f t="shared" si="921"/>
         <v>-1</v>
       </c>
       <c r="CE425" s="40">
@@ -83502,11 +83492,11 @@
         <v>15</v>
       </c>
       <c r="D426" s="35">
-        <f t="shared" ref="D426:E426" si="923">D425</f>
+        <f t="shared" ref="D426:E426" si="922">D425</f>
         <v>2025</v>
       </c>
       <c r="E426" s="40" t="str">
-        <f t="shared" si="923"/>
+        <f t="shared" si="922"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F426" s="2">
@@ -83616,11 +83606,11 @@
         <v>5016</v>
       </c>
       <c r="AO426" s="40">
-        <f t="shared" ref="AO426:AP426" si="924">AO425</f>
+        <f t="shared" ref="AO426:AP426" si="923">AO425</f>
         <v>0.7</v>
       </c>
       <c r="AP426" s="40" t="str">
-        <f t="shared" si="924"/>
+        <f t="shared" si="923"/>
         <v>Yes</v>
       </c>
       <c r="AQ426" s="138">
@@ -83681,9 +83671,8 @@
       <c r="BI426" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ426" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ426" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK426" s="2" t="s">
         <v>376</v>
@@ -83731,23 +83720,23 @@
         <v>274</v>
       </c>
       <c r="BZ426" s="124" t="str">
-        <f t="shared" ref="BZ426:CD426" si="925">BZ425</f>
+        <f t="shared" ref="BZ426:CD426" si="924">BZ425</f>
         <v>not compact</v>
       </c>
       <c r="CA426" s="69" t="str">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>not compact</v>
       </c>
       <c r="CB426" s="35" t="str">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC426" s="35" t="str">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>Standard</v>
       </c>
       <c r="CD426" s="40">
-        <f t="shared" si="925"/>
+        <f t="shared" si="924"/>
         <v>-1</v>
       </c>
       <c r="CE426" s="40">
@@ -83777,11 +83766,11 @@
         <v>16</v>
       </c>
       <c r="D427" s="35">
-        <f t="shared" ref="D427:E427" si="926">D426</f>
+        <f t="shared" ref="D427:E427" si="925">D426</f>
         <v>2025</v>
       </c>
       <c r="E427" s="40" t="str">
-        <f t="shared" si="926"/>
+        <f t="shared" si="925"/>
         <v>LowRiseRes</v>
       </c>
       <c r="F427" s="2">
@@ -83891,11 +83880,11 @@
         <v>10016</v>
       </c>
       <c r="AO427" s="40">
-        <f t="shared" ref="AO427:AP427" si="927">AO426</f>
+        <f t="shared" ref="AO427:AP427" si="926">AO426</f>
         <v>0.7</v>
       </c>
       <c r="AP427" s="40" t="str">
-        <f t="shared" si="927"/>
+        <f t="shared" si="926"/>
         <v>Yes</v>
       </c>
       <c r="AQ427" s="138">
@@ -83956,9 +83945,8 @@
       <c r="BI427" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="BJ427" s="35" t="str">
-        <f t="shared" si="890"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ427" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK427" s="2" t="s">
         <v>375</v>
@@ -84006,23 +83994,23 @@
         <v>274</v>
       </c>
       <c r="BZ427" s="124" t="str">
-        <f t="shared" ref="BZ427:CD427" si="928">BZ426</f>
+        <f t="shared" ref="BZ427:CD427" si="927">BZ426</f>
         <v>not compact</v>
       </c>
       <c r="CA427" s="69" t="str">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>not compact</v>
       </c>
       <c r="CB427" s="35" t="str">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC427" s="35" t="str">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>Standard</v>
       </c>
       <c r="CD427" s="40">
-        <f t="shared" si="928"/>
+        <f t="shared" si="927"/>
         <v>-1</v>
       </c>
       <c r="CE427" s="121">
@@ -84125,18 +84113,18 @@
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB428" s="140">
-        <f t="shared" ref="AB428:AB443" si="929">AB412</f>
+        <f t="shared" ref="AB428:AB443" si="928">AB412</f>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC428" s="144">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD428" s="144">
-        <f t="shared" ref="AD428:AE428" si="930">AD412</f>
+        <f t="shared" ref="AD428:AE428" si="929">AD412</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE428" s="144">
-        <f t="shared" si="930"/>
+        <f t="shared" si="929"/>
         <v>0.253</v>
       </c>
       <c r="AF428" s="140">
@@ -84229,22 +84217,22 @@
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH428" s="145" t="str">
-        <f t="shared" ref="BH428:BI428" si="931">BH412</f>
+        <f t="shared" ref="BH428:BI428" si="930">BH412</f>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI428" s="145" t="str">
+        <f t="shared" si="930"/>
+        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
+      </c>
+      <c r="BJ428" s="140" t="s">
+        <v>338</v>
+      </c>
+      <c r="BK428" s="145" t="str">
+        <f t="shared" ref="BK428:BL428" si="931">BK412</f>
+        <v>T24-2022 ExtWall 6in Conc R13</v>
+      </c>
+      <c r="BL428" s="145" t="str">
         <f t="shared" si="931"/>
-        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
-      </c>
-      <c r="BJ428" s="140" t="s">
-        <v>203</v>
-      </c>
-      <c r="BK428" s="145" t="str">
-        <f t="shared" ref="BK428:BL428" si="932">BK412</f>
-        <v>T24-2022 ExtWall 6in Conc R13</v>
-      </c>
-      <c r="BL428" s="145" t="str">
-        <f t="shared" si="932"/>
         <v>T24-2022 ExtWall 8in Conc U=0.253</v>
       </c>
       <c r="BM428" s="140" t="s">
@@ -84332,7 +84320,7 @@
         <v>2025</v>
       </c>
       <c r="E429" s="40" t="str">
-        <f t="shared" ref="E429" si="933">E428</f>
+        <f t="shared" ref="E429" si="932">E428</f>
         <v>HiRiseRes</v>
       </c>
       <c r="F429" s="2">
@@ -84400,22 +84388,22 @@
         <v>15</v>
       </c>
       <c r="AA429" s="2">
-        <f t="shared" ref="AA429:AA443" si="934">AA413</f>
+        <f t="shared" ref="AA429:AA443" si="933">AA413</f>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB429" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC429" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD429" s="120">
-        <f t="shared" ref="AD429:AE429" si="935">AD413</f>
+        <f t="shared" ref="AD429:AE429" si="934">AD413</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE429" s="120">
-        <f t="shared" si="935"/>
+        <f t="shared" si="934"/>
         <v>0.65</v>
       </c>
       <c r="AF429" s="2">
@@ -84507,27 +84495,26 @@
         <v>0</v>
       </c>
       <c r="BG429" s="138" t="str">
-        <f t="shared" ref="BG429:BI443" si="936">BG413</f>
+        <f t="shared" ref="BG429:BI443" si="935">BG413</f>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH429" s="138" t="str">
+        <f t="shared" si="935"/>
+        <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
+      </c>
+      <c r="BI429" s="138" t="str">
+        <f t="shared" si="935"/>
+        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
+      </c>
+      <c r="BJ429" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="BK429" s="138" t="str">
+        <f t="shared" ref="BK429:BL429" si="936">BK413</f>
+        <v>T24-2022 ExtWall 6in Conc R13</v>
+      </c>
+      <c r="BL429" s="138" t="str">
         <f t="shared" si="936"/>
-        <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
-      </c>
-      <c r="BI429" s="138" t="str">
-        <f t="shared" si="936"/>
-        <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
-      </c>
-      <c r="BJ429" s="35" t="str">
-        <f>BJ428</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
-      </c>
-      <c r="BK429" s="138" t="str">
-        <f t="shared" ref="BK429:BL429" si="937">BK413</f>
-        <v>T24-2022 ExtWall 6in Conc R13</v>
-      </c>
-      <c r="BL429" s="138" t="str">
-        <f t="shared" si="937"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM429" s="2" t="s">
@@ -84616,11 +84603,11 @@
         <v>3</v>
       </c>
       <c r="D430" s="35">
-        <f t="shared" ref="D430:E430" si="938">D429</f>
+        <f t="shared" ref="D430:E430" si="937">D429</f>
         <v>2025</v>
       </c>
       <c r="E430" s="40" t="str">
-        <f t="shared" si="938"/>
+        <f t="shared" si="937"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F430" s="2">
@@ -84666,7 +84653,7 @@
         <v>0.62</v>
       </c>
       <c r="T430" s="35">
-        <f t="shared" ref="T430:T443" si="939">T429</f>
+        <f t="shared" ref="T430:T443" si="938">T429</f>
         <v>7</v>
       </c>
       <c r="U430" s="38">
@@ -84688,22 +84675,22 @@
         <v>15</v>
       </c>
       <c r="AA430" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB430" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC430" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD430" s="120">
-        <f t="shared" ref="AD430:AE430" si="940">AD414</f>
+        <f t="shared" ref="AD430:AE430" si="939">AD414</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE430" s="120">
-        <f t="shared" si="940"/>
+        <f t="shared" si="939"/>
         <v>0.65</v>
       </c>
       <c r="AF430" s="2">
@@ -84734,33 +84721,33 @@
         <v>5016</v>
       </c>
       <c r="AO430" s="40">
-        <f t="shared" ref="AO430:AP430" si="941">AO429</f>
+        <f t="shared" ref="AO430:AP430" si="940">AO429</f>
         <v>0.7</v>
       </c>
       <c r="AP430" s="40" t="str">
-        <f t="shared" si="941"/>
+        <f t="shared" si="940"/>
         <v>Yes</v>
       </c>
       <c r="AQ430" s="138">
-        <f t="shared" ref="AQ430:AS430" si="942">AQ414</f>
+        <f t="shared" ref="AQ430" si="941">AQ414</f>
         <v>0.41</v>
       </c>
       <c r="AR430" s="138">
         <v>0.26</v>
       </c>
       <c r="AS430" s="138">
-        <f t="shared" ref="AS430:AU443" si="943">AS414</f>
+        <f t="shared" ref="AS430:AT443" si="942">AS414</f>
         <v>0.46</v>
       </c>
       <c r="AT430" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU430" s="138">
         <v>0.24</v>
       </c>
       <c r="AV430" s="138">
-        <f t="shared" ref="AV430:AV443" si="944">AV414</f>
+        <f t="shared" ref="AV430:AV443" si="943">AV414</f>
         <v>0.37</v>
       </c>
       <c r="AW430" s="38">
@@ -84791,31 +84778,30 @@
         <v>114</v>
       </c>
       <c r="BF430" s="40">
-        <f t="shared" ref="BF430:BF443" si="945">BF429</f>
+        <f t="shared" ref="BF430:BF443" si="944">BF429</f>
         <v>0</v>
       </c>
       <c r="BG430" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH430" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI430" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ430" s="35" t="str">
-        <f t="shared" ref="BJ430:BJ443" si="946">BJ429</f>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ430" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK430" s="138" t="str">
-        <f t="shared" ref="BK430:BL430" si="947">BK414</f>
+        <f t="shared" ref="BK430:BL430" si="945">BK414</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL430" s="138" t="str">
-        <f t="shared" si="947"/>
+        <f t="shared" si="945"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM430" s="2" t="s">
@@ -84858,23 +84844,23 @@
         <v>273</v>
       </c>
       <c r="BZ430" s="124" t="str">
-        <f t="shared" ref="BZ430:CD430" si="948">BZ429</f>
+        <f t="shared" ref="BZ430:CD430" si="946">BZ429</f>
         <v>not compact</v>
       </c>
       <c r="CA430" s="69" t="str">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>not compact</v>
       </c>
       <c r="CB430" s="35" t="str">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC430" s="35" t="str">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>Standard</v>
       </c>
       <c r="CD430" s="40">
-        <f t="shared" si="948"/>
+        <f t="shared" si="946"/>
         <v>-1</v>
       </c>
       <c r="CE430" s="40">
@@ -84904,11 +84890,11 @@
         <v>4</v>
       </c>
       <c r="D431" s="35">
-        <f t="shared" ref="D431:E431" si="949">D430</f>
+        <f t="shared" ref="D431:E431" si="947">D430</f>
         <v>2025</v>
       </c>
       <c r="E431" s="40" t="str">
-        <f t="shared" si="949"/>
+        <f t="shared" si="947"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F431" s="2">
@@ -84954,7 +84940,7 @@
         <v>0.62</v>
       </c>
       <c r="T431" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U431" s="38">
@@ -84976,22 +84962,22 @@
         <v>15</v>
       </c>
       <c r="AA431" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB431" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC431" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD431" s="120">
-        <f t="shared" ref="AD431:AE431" si="950">AD415</f>
+        <f t="shared" ref="AD431:AE431" si="948">AD415</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE431" s="120">
-        <f t="shared" si="950"/>
+        <f t="shared" si="948"/>
         <v>0.65</v>
       </c>
       <c r="AF431" s="2">
@@ -85022,33 +85008,33 @@
         <v>5016</v>
       </c>
       <c r="AO431" s="40">
-        <f t="shared" ref="AO431:AP431" si="951">AO430</f>
+        <f t="shared" ref="AO431:AP431" si="949">AO430</f>
         <v>0.7</v>
       </c>
       <c r="AP431" s="40" t="str">
-        <f t="shared" si="951"/>
+        <f t="shared" si="949"/>
         <v>Yes</v>
       </c>
       <c r="AQ431" s="138">
-        <f t="shared" ref="AQ431:AS431" si="952">AQ415</f>
+        <f t="shared" ref="AQ431" si="950">AQ415</f>
         <v>0.41</v>
       </c>
       <c r="AR431" s="138">
         <v>0.26</v>
       </c>
       <c r="AS431" s="138">
-        <f t="shared" ref="AS431:AU431" si="953">AS415</f>
+        <f t="shared" ref="AS431" si="951">AS415</f>
         <v>0.46</v>
       </c>
       <c r="AT431" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU431" s="138">
         <v>0.24</v>
       </c>
       <c r="AV431" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW431" s="38">
@@ -85079,31 +85065,30 @@
         <v>114</v>
       </c>
       <c r="BF431" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG431" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH431" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI431" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ431" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ431" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK431" s="138" t="str">
-        <f t="shared" ref="BK431:BL431" si="954">BK415</f>
+        <f t="shared" ref="BK431:BL431" si="952">BK415</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL431" s="138" t="str">
-        <f t="shared" si="954"/>
+        <f t="shared" si="952"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM431" s="2" t="s">
@@ -85146,23 +85131,23 @@
         <v>274</v>
       </c>
       <c r="BZ431" s="124" t="str">
-        <f t="shared" ref="BZ431:CD431" si="955">BZ430</f>
+        <f t="shared" ref="BZ431:CD431" si="953">BZ430</f>
         <v>not compact</v>
       </c>
       <c r="CA431" s="69" t="str">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>not compact</v>
       </c>
       <c r="CB431" s="35" t="str">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC431" s="35" t="str">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>Standard</v>
       </c>
       <c r="CD431" s="40">
-        <f t="shared" si="955"/>
+        <f t="shared" si="953"/>
         <v>-1</v>
       </c>
       <c r="CE431" s="40">
@@ -85192,11 +85177,11 @@
         <v>5</v>
       </c>
       <c r="D432" s="35">
-        <f t="shared" ref="D432:E432" si="956">D431</f>
+        <f t="shared" ref="D432:E432" si="954">D431</f>
         <v>2025</v>
       </c>
       <c r="E432" s="40" t="str">
-        <f t="shared" si="956"/>
+        <f t="shared" si="954"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F432" s="2">
@@ -85242,7 +85227,7 @@
         <v>0.62</v>
       </c>
       <c r="T432" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U432" s="38">
@@ -85264,22 +85249,22 @@
         <v>15</v>
       </c>
       <c r="AA432" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB432" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC432" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD432" s="120">
-        <f t="shared" ref="AD432:AE432" si="957">AD416</f>
+        <f t="shared" ref="AD432:AE432" si="955">AD416</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE432" s="120">
-        <f t="shared" si="957"/>
+        <f t="shared" si="955"/>
         <v>0.65</v>
       </c>
       <c r="AF432" s="2">
@@ -85310,33 +85295,33 @@
         <v>5016</v>
       </c>
       <c r="AO432" s="40">
-        <f t="shared" ref="AO432:AP432" si="958">AO431</f>
+        <f t="shared" ref="AO432:AP432" si="956">AO431</f>
         <v>0.7</v>
       </c>
       <c r="AP432" s="40" t="str">
-        <f t="shared" si="958"/>
+        <f t="shared" si="956"/>
         <v>Yes</v>
       </c>
       <c r="AQ432" s="138">
-        <f t="shared" ref="AQ432:AS432" si="959">AQ416</f>
+        <f t="shared" ref="AQ432" si="957">AQ416</f>
         <v>0.41</v>
       </c>
       <c r="AR432" s="138">
         <v>0.26</v>
       </c>
       <c r="AS432" s="138">
-        <f t="shared" ref="AS432:AU432" si="960">AS416</f>
+        <f t="shared" ref="AS432" si="958">AS416</f>
         <v>0.46</v>
       </c>
       <c r="AT432" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU432" s="138">
         <v>0.24</v>
       </c>
       <c r="AV432" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW432" s="38">
@@ -85367,31 +85352,30 @@
         <v>114</v>
       </c>
       <c r="BF432" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG432" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH432" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI432" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ432" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ432" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK432" s="138" t="str">
-        <f t="shared" ref="BK432:BL432" si="961">BK416</f>
+        <f t="shared" ref="BK432:BL432" si="959">BK416</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL432" s="138" t="str">
-        <f t="shared" si="961"/>
+        <f t="shared" si="959"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM432" s="2" t="s">
@@ -85434,23 +85418,23 @@
         <v>273</v>
       </c>
       <c r="BZ432" s="124" t="str">
-        <f t="shared" ref="BZ432:CD432" si="962">BZ431</f>
+        <f t="shared" ref="BZ432:CD432" si="960">BZ431</f>
         <v>not compact</v>
       </c>
       <c r="CA432" s="69" t="str">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>not compact</v>
       </c>
       <c r="CB432" s="35" t="str">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC432" s="35" t="str">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>Standard</v>
       </c>
       <c r="CD432" s="40">
-        <f t="shared" si="962"/>
+        <f t="shared" si="960"/>
         <v>-1</v>
       </c>
       <c r="CE432" s="40">
@@ -85480,11 +85464,11 @@
         <v>6</v>
       </c>
       <c r="D433" s="35">
-        <f t="shared" ref="D433:E433" si="963">D432</f>
+        <f t="shared" ref="D433:E433" si="961">D432</f>
         <v>2025</v>
       </c>
       <c r="E433" s="40" t="str">
-        <f t="shared" si="963"/>
+        <f t="shared" si="961"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F433" s="2">
@@ -85530,7 +85514,7 @@
         <v>0.62</v>
       </c>
       <c r="T433" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U433" s="38">
@@ -85552,22 +85536,22 @@
         <v>15</v>
       </c>
       <c r="AA433" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB433" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AC433" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AD433" s="2">
-        <f t="shared" ref="AD433:AE433" si="964">AD417</f>
+        <f t="shared" ref="AD433:AE433" si="962">AD417</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE433" s="2">
-        <f t="shared" si="964"/>
+        <f t="shared" si="962"/>
         <v>0.69</v>
       </c>
       <c r="AF433" s="2">
@@ -85598,33 +85582,33 @@
         <v>5016</v>
       </c>
       <c r="AO433" s="40">
-        <f t="shared" ref="AO433:AP433" si="965">AO432</f>
+        <f t="shared" ref="AO433:AP433" si="963">AO432</f>
         <v>0.7</v>
       </c>
       <c r="AP433" s="40" t="str">
-        <f t="shared" si="965"/>
+        <f t="shared" si="963"/>
         <v>Yes</v>
       </c>
       <c r="AQ433" s="138">
-        <f t="shared" ref="AQ433:AS433" si="966">AQ417</f>
+        <f t="shared" ref="AQ433" si="964">AQ417</f>
         <v>0.41</v>
       </c>
       <c r="AR433" s="138">
         <v>0.26</v>
       </c>
       <c r="AS433" s="138">
-        <f t="shared" ref="AS433:AU433" si="967">AS417</f>
+        <f t="shared" ref="AS433" si="965">AS417</f>
         <v>0.46</v>
       </c>
       <c r="AT433" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU433" s="138">
         <v>0.24</v>
       </c>
       <c r="AV433" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW433" s="38">
@@ -85655,30 +85639,30 @@
         <v>114</v>
       </c>
       <c r="BF433" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG433" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH433" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BI433" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BJ433" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK433" s="138" t="str">
-        <f t="shared" ref="BK433:BL433" si="968">BK417</f>
+        <f t="shared" ref="BK433:BL433" si="966">BK417</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL433" s="138" t="str">
-        <f t="shared" si="968"/>
+        <f t="shared" si="966"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM433" s="2" t="s">
@@ -85721,23 +85705,23 @@
         <v>274</v>
       </c>
       <c r="BZ433" s="124" t="str">
-        <f t="shared" ref="BZ433:CD433" si="969">BZ432</f>
+        <f t="shared" ref="BZ433:CD433" si="967">BZ432</f>
         <v>not compact</v>
       </c>
       <c r="CA433" s="69" t="str">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>not compact</v>
       </c>
       <c r="CB433" s="35" t="str">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC433" s="35" t="str">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>Standard</v>
       </c>
       <c r="CD433" s="40">
-        <f t="shared" si="969"/>
+        <f t="shared" si="967"/>
         <v>-1</v>
       </c>
       <c r="CE433" s="40">
@@ -85767,11 +85751,11 @@
         <v>7</v>
       </c>
       <c r="D434" s="35">
-        <f t="shared" ref="D434:E434" si="970">D433</f>
+        <f t="shared" ref="D434:E434" si="968">D433</f>
         <v>2025</v>
       </c>
       <c r="E434" s="40" t="str">
-        <f t="shared" si="970"/>
+        <f t="shared" si="968"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F434" s="2">
@@ -85817,7 +85801,7 @@
         <v>0.62</v>
       </c>
       <c r="T434" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U434" s="38">
@@ -85839,22 +85823,22 @@
         <v>15</v>
       </c>
       <c r="AA434" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB434" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AC434" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AD434" s="2">
-        <f t="shared" ref="AD434:AE434" si="971">AD418</f>
+        <f t="shared" ref="AD434:AE434" si="969">AD418</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE434" s="2">
-        <f t="shared" si="971"/>
+        <f t="shared" si="969"/>
         <v>0.69</v>
       </c>
       <c r="AF434" s="2">
@@ -85885,32 +85869,32 @@
         <v>5016</v>
       </c>
       <c r="AO434" s="40">
-        <f t="shared" ref="AO434:AP434" si="972">AO433</f>
+        <f t="shared" ref="AO434" si="970">AO433</f>
         <v>0.7</v>
       </c>
       <c r="AP434" s="121" t="s">
         <v>292</v>
       </c>
       <c r="AQ434" s="138">
-        <f t="shared" ref="AQ434:AS434" si="973">AQ418</f>
+        <f t="shared" ref="AQ434" si="971">AQ418</f>
         <v>0.41</v>
       </c>
       <c r="AR434" s="138">
         <v>0.26</v>
       </c>
       <c r="AS434" s="138">
-        <f t="shared" ref="AS434:AU434" si="974">AS418</f>
+        <f t="shared" ref="AS434" si="972">AS418</f>
         <v>0.46</v>
       </c>
       <c r="AT434" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU434" s="138">
         <v>0.24</v>
       </c>
       <c r="AV434" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW434" s="38">
@@ -85941,30 +85925,30 @@
         <v>114</v>
       </c>
       <c r="BF434" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG434" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH434" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BI434" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.065</v>
       </c>
       <c r="BJ434" s="126" t="s">
-        <v>126</v>
+        <v>338</v>
       </c>
       <c r="BK434" s="138" t="str">
-        <f t="shared" ref="BK434:BL434" si="975">BK418</f>
+        <f t="shared" ref="BK434:BL434" si="973">BK418</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL434" s="138" t="str">
-        <f t="shared" si="975"/>
+        <f t="shared" si="973"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM434" s="2" t="s">
@@ -86007,23 +85991,23 @@
         <v>274</v>
       </c>
       <c r="BZ434" s="124" t="str">
-        <f t="shared" ref="BZ434:CD434" si="976">BZ433</f>
+        <f t="shared" ref="BZ434:CD434" si="974">BZ433</f>
         <v>not compact</v>
       </c>
       <c r="CA434" s="69" t="str">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>not compact</v>
       </c>
       <c r="CB434" s="35" t="str">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC434" s="35" t="str">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>Standard</v>
       </c>
       <c r="CD434" s="40">
-        <f t="shared" si="976"/>
+        <f t="shared" si="974"/>
         <v>-1</v>
       </c>
       <c r="CE434" s="40">
@@ -86053,11 +86037,11 @@
         <v>8</v>
       </c>
       <c r="D435" s="35">
-        <f t="shared" ref="D435:E435" si="977">D434</f>
+        <f t="shared" ref="D435:E435" si="975">D434</f>
         <v>2025</v>
       </c>
       <c r="E435" s="40" t="str">
-        <f t="shared" si="977"/>
+        <f t="shared" si="975"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F435" s="2">
@@ -86103,7 +86087,7 @@
         <v>0.62</v>
       </c>
       <c r="T435" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U435" s="38">
@@ -86125,22 +86109,22 @@
         <v>15</v>
       </c>
       <c r="AA435" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB435" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC435" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD435" s="120">
-        <f t="shared" ref="AD435:AE435" si="978">AD419</f>
+        <f t="shared" ref="AD435:AE435" si="976">AD419</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE435" s="120">
-        <f t="shared" si="978"/>
+        <f t="shared" si="976"/>
         <v>0.69</v>
       </c>
       <c r="AF435" s="2">
@@ -86171,32 +86155,32 @@
         <v>5016</v>
       </c>
       <c r="AO435" s="40">
-        <f t="shared" ref="AO435:AP435" si="979">AO434</f>
+        <f t="shared" ref="AO435" si="977">AO434</f>
         <v>0.7</v>
       </c>
       <c r="AP435" s="38" t="s">
         <v>291</v>
       </c>
       <c r="AQ435" s="138">
-        <f t="shared" ref="AQ435:AS435" si="980">AQ419</f>
+        <f t="shared" ref="AQ435" si="978">AQ419</f>
         <v>0.41</v>
       </c>
       <c r="AR435" s="138">
         <v>0.26</v>
       </c>
       <c r="AS435" s="138">
-        <f t="shared" ref="AS435:AU435" si="981">AS419</f>
+        <f t="shared" ref="AS435" si="979">AS419</f>
         <v>0.46</v>
       </c>
       <c r="AT435" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU435" s="138">
         <v>0.24</v>
       </c>
       <c r="AV435" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW435" s="38">
@@ -86227,30 +86211,30 @@
         <v>114</v>
       </c>
       <c r="BF435" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG435" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH435" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI435" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BJ435" s="2" t="s">
-        <v>203</v>
+        <v>338</v>
       </c>
       <c r="BK435" s="138" t="str">
-        <f t="shared" ref="BK435:BL435" si="982">BK419</f>
+        <f t="shared" ref="BK435:BL435" si="980">BK419</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL435" s="138" t="str">
-        <f t="shared" si="982"/>
+        <f t="shared" si="980"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM435" s="2" t="s">
@@ -86293,23 +86277,23 @@
         <v>274</v>
       </c>
       <c r="BZ435" s="124" t="str">
-        <f t="shared" ref="BZ435:CD435" si="983">BZ434</f>
+        <f t="shared" ref="BZ435:CD435" si="981">BZ434</f>
         <v>not compact</v>
       </c>
       <c r="CA435" s="69" t="str">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>not compact</v>
       </c>
       <c r="CB435" s="35" t="str">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC435" s="35" t="str">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>Standard</v>
       </c>
       <c r="CD435" s="40">
-        <f t="shared" si="983"/>
+        <f t="shared" si="981"/>
         <v>-1</v>
       </c>
       <c r="CE435" s="40">
@@ -86339,11 +86323,11 @@
         <v>9</v>
       </c>
       <c r="D436" s="35">
-        <f t="shared" ref="D436:E436" si="984">D435</f>
+        <f t="shared" ref="D436:E436" si="982">D435</f>
         <v>2025</v>
       </c>
       <c r="E436" s="40" t="str">
-        <f t="shared" si="984"/>
+        <f t="shared" si="982"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F436" s="2">
@@ -86389,7 +86373,7 @@
         <v>0.62</v>
       </c>
       <c r="T436" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U436" s="38">
@@ -86411,22 +86395,22 @@
         <v>15</v>
       </c>
       <c r="AA436" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB436" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC436" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD436" s="120">
-        <f t="shared" ref="AD436:AE436" si="985">AD420</f>
+        <f t="shared" ref="AD436:AE436" si="983">AD420</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE436" s="120">
-        <f t="shared" si="985"/>
+        <f t="shared" si="983"/>
         <v>0.69</v>
       </c>
       <c r="AF436" s="2">
@@ -86457,33 +86441,33 @@
         <v>5016</v>
       </c>
       <c r="AO436" s="40">
-        <f t="shared" ref="AO436:AP436" si="986">AO435</f>
+        <f t="shared" ref="AO436:AP436" si="984">AO435</f>
         <v>0.7</v>
       </c>
       <c r="AP436" s="40" t="str">
-        <f t="shared" si="986"/>
+        <f t="shared" si="984"/>
         <v>Yes</v>
       </c>
       <c r="AQ436" s="138">
-        <f t="shared" ref="AQ436:AS436" si="987">AQ420</f>
+        <f t="shared" ref="AQ436" si="985">AQ420</f>
         <v>0.41</v>
       </c>
       <c r="AR436" s="138">
         <v>0.26</v>
       </c>
       <c r="AS436" s="138">
-        <f t="shared" ref="AS436:AU436" si="988">AS420</f>
+        <f t="shared" ref="AS436" si="986">AS420</f>
         <v>0.46</v>
       </c>
       <c r="AT436" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU436" s="138">
         <v>0.24</v>
       </c>
       <c r="AV436" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW436" s="38">
@@ -86514,31 +86498,30 @@
         <v>114</v>
       </c>
       <c r="BF436" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG436" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH436" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI436" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ436" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ436" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK436" s="138" t="str">
-        <f t="shared" ref="BK436:BL436" si="989">BK420</f>
+        <f t="shared" ref="BK436:BL436" si="987">BK420</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL436" s="138" t="str">
-        <f t="shared" si="989"/>
+        <f t="shared" si="987"/>
         <v>T24-2022 ExtWall 7in Conc U=0.690</v>
       </c>
       <c r="BM436" s="2" t="s">
@@ -86581,23 +86564,23 @@
         <v>274</v>
       </c>
       <c r="BZ436" s="124" t="str">
-        <f t="shared" ref="BZ436:CD436" si="990">BZ435</f>
+        <f t="shared" ref="BZ436:CD436" si="988">BZ435</f>
         <v>not compact</v>
       </c>
       <c r="CA436" s="69" t="str">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>not compact</v>
       </c>
       <c r="CB436" s="35" t="str">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC436" s="35" t="str">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>Standard</v>
       </c>
       <c r="CD436" s="40">
-        <f t="shared" si="990"/>
+        <f t="shared" si="988"/>
         <v>-1</v>
       </c>
       <c r="CE436" s="40">
@@ -86627,11 +86610,11 @@
         <v>10</v>
       </c>
       <c r="D437" s="35">
-        <f t="shared" ref="D437:E437" si="991">D436</f>
+        <f t="shared" ref="D437:E437" si="989">D436</f>
         <v>2025</v>
       </c>
       <c r="E437" s="40" t="str">
-        <f t="shared" si="991"/>
+        <f t="shared" si="989"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F437" s="2">
@@ -86677,7 +86660,7 @@
         <v>0.62</v>
       </c>
       <c r="T437" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U437" s="38">
@@ -86699,22 +86682,22 @@
         <v>15</v>
       </c>
       <c r="AA437" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="AB437" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC437" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD437" s="120">
-        <f t="shared" ref="AD437:AE437" si="992">AD421</f>
+        <f t="shared" ref="AD437:AE437" si="990">AD421</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE437" s="120">
-        <f t="shared" si="992"/>
+        <f t="shared" si="990"/>
         <v>0.65</v>
       </c>
       <c r="AF437" s="2">
@@ -86745,33 +86728,33 @@
         <v>5016</v>
       </c>
       <c r="AO437" s="40">
-        <f t="shared" ref="AO437:AP437" si="993">AO436</f>
+        <f t="shared" ref="AO437:AP437" si="991">AO436</f>
         <v>0.7</v>
       </c>
       <c r="AP437" s="40" t="str">
-        <f t="shared" si="993"/>
+        <f t="shared" si="991"/>
         <v>Yes</v>
       </c>
       <c r="AQ437" s="138">
-        <f t="shared" ref="AQ437:AS437" si="994">AQ421</f>
+        <f t="shared" ref="AQ437" si="992">AQ421</f>
         <v>0.41</v>
       </c>
       <c r="AR437" s="138">
         <v>0.26</v>
       </c>
       <c r="AS437" s="138">
-        <f t="shared" ref="AS437:AU437" si="995">AS421</f>
+        <f t="shared" ref="AS437" si="993">AS421</f>
         <v>0.46</v>
       </c>
       <c r="AT437" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU437" s="138">
         <v>0.24</v>
       </c>
       <c r="AV437" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW437" s="38">
@@ -86802,31 +86785,30 @@
         <v>114</v>
       </c>
       <c r="BF437" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG437" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.061</v>
       </c>
       <c r="BH437" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI437" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ437" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ437" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK437" s="138" t="str">
-        <f t="shared" ref="BK437:BL437" si="996">BK421</f>
+        <f t="shared" ref="BK437:BL437" si="994">BK421</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL437" s="138" t="str">
-        <f t="shared" si="996"/>
+        <f t="shared" si="994"/>
         <v>T24-2022 ExtWall 8in Conc U=0.650</v>
       </c>
       <c r="BM437" s="2" t="s">
@@ -86869,23 +86851,23 @@
         <v>274</v>
       </c>
       <c r="BZ437" s="124" t="str">
-        <f t="shared" ref="BZ437:CD437" si="997">BZ436</f>
+        <f t="shared" ref="BZ437:CD437" si="995">BZ436</f>
         <v>not compact</v>
       </c>
       <c r="CA437" s="69" t="str">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>not compact</v>
       </c>
       <c r="CB437" s="35" t="str">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC437" s="35" t="str">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>Standard</v>
       </c>
       <c r="CD437" s="40">
-        <f t="shared" si="997"/>
+        <f t="shared" si="995"/>
         <v>-1</v>
       </c>
       <c r="CE437" s="40">
@@ -86915,11 +86897,11 @@
         <v>11</v>
       </c>
       <c r="D438" s="35">
-        <f t="shared" ref="D438:E438" si="998">D437</f>
+        <f t="shared" ref="D438:E438" si="996">D437</f>
         <v>2025</v>
       </c>
       <c r="E438" s="40" t="str">
-        <f t="shared" si="998"/>
+        <f t="shared" si="996"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F438" s="2">
@@ -86965,7 +86947,7 @@
         <v>0.62</v>
       </c>
       <c r="T438" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U438" s="38">
@@ -86987,22 +86969,22 @@
         <v>15</v>
       </c>
       <c r="AA438" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB438" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC438" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD438" s="120">
-        <f t="shared" ref="AD438:AE438" si="999">AD422</f>
+        <f t="shared" ref="AD438:AE438" si="997">AD422</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE438" s="120">
-        <f t="shared" si="999"/>
+        <f t="shared" si="997"/>
         <v>0.184</v>
       </c>
       <c r="AF438" s="2">
@@ -87033,33 +87015,33 @@
         <v>5016</v>
       </c>
       <c r="AO438" s="40">
-        <f t="shared" ref="AO438:AP438" si="1000">AO437</f>
+        <f t="shared" ref="AO438:AP438" si="998">AO437</f>
         <v>0.7</v>
       </c>
       <c r="AP438" s="40" t="str">
-        <f t="shared" si="1000"/>
+        <f t="shared" si="998"/>
         <v>Yes</v>
       </c>
       <c r="AQ438" s="138">
-        <f t="shared" ref="AQ438:AS438" si="1001">AQ422</f>
+        <f t="shared" ref="AQ438" si="999">AQ422</f>
         <v>0.41</v>
       </c>
       <c r="AR438" s="138">
         <v>0.26</v>
       </c>
       <c r="AS438" s="138">
-        <f t="shared" ref="AS438:AU438" si="1002">AS422</f>
+        <f t="shared" ref="AS438" si="1000">AS422</f>
         <v>0.46</v>
       </c>
       <c r="AT438" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU438" s="138">
         <v>0.24</v>
       </c>
       <c r="AV438" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW438" s="38">
@@ -87090,31 +87072,30 @@
         <v>114</v>
       </c>
       <c r="BF438" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG438" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH438" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI438" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ438" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ438" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK438" s="138" t="str">
-        <f t="shared" ref="BK438:BL438" si="1003">BK422</f>
+        <f t="shared" ref="BK438:BL438" si="1001">BK422</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL438" s="138" t="str">
-        <f t="shared" si="1003"/>
+        <f t="shared" si="1001"/>
         <v>T24-2022 ExtWall 8in Conc U=0.184</v>
       </c>
       <c r="BM438" s="2" t="s">
@@ -87157,23 +87138,23 @@
         <v>274</v>
       </c>
       <c r="BZ438" s="124" t="str">
-        <f t="shared" ref="BZ438:CD438" si="1004">BZ437</f>
+        <f t="shared" ref="BZ438:CD438" si="1002">BZ437</f>
         <v>not compact</v>
       </c>
       <c r="CA438" s="69" t="str">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>not compact</v>
       </c>
       <c r="CB438" s="35" t="str">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC438" s="35" t="str">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>Standard</v>
       </c>
       <c r="CD438" s="40">
-        <f t="shared" si="1004"/>
+        <f t="shared" si="1002"/>
         <v>-1</v>
       </c>
       <c r="CE438" s="40">
@@ -87203,11 +87184,11 @@
         <v>12</v>
       </c>
       <c r="D439" s="35">
-        <f t="shared" ref="D439:E439" si="1005">D438</f>
+        <f t="shared" ref="D439:E439" si="1003">D438</f>
         <v>2025</v>
       </c>
       <c r="E439" s="40" t="str">
-        <f t="shared" si="1005"/>
+        <f t="shared" si="1003"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F439" s="2">
@@ -87253,7 +87234,7 @@
         <v>0.62</v>
       </c>
       <c r="T439" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U439" s="38">
@@ -87275,22 +87256,22 @@
         <v>15</v>
       </c>
       <c r="AA439" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB439" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC439" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD439" s="120">
-        <f t="shared" ref="AD439:AE439" si="1006">AD423</f>
+        <f t="shared" ref="AD439:AE439" si="1004">AD423</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE439" s="120">
-        <f t="shared" si="1006"/>
+        <f t="shared" si="1004"/>
         <v>0.253</v>
       </c>
       <c r="AF439" s="2">
@@ -87321,33 +87302,33 @@
         <v>5016</v>
       </c>
       <c r="AO439" s="40">
-        <f t="shared" ref="AO439:AP439" si="1007">AO438</f>
+        <f t="shared" ref="AO439:AP439" si="1005">AO438</f>
         <v>0.7</v>
       </c>
       <c r="AP439" s="40" t="str">
-        <f t="shared" si="1007"/>
+        <f t="shared" si="1005"/>
         <v>Yes</v>
       </c>
       <c r="AQ439" s="138">
-        <f t="shared" ref="AQ439:AS439" si="1008">AQ423</f>
+        <f t="shared" ref="AQ439" si="1006">AQ423</f>
         <v>0.41</v>
       </c>
       <c r="AR439" s="138">
         <v>0.26</v>
       </c>
       <c r="AS439" s="138">
-        <f t="shared" ref="AS439:AU439" si="1009">AS423</f>
+        <f t="shared" ref="AS439" si="1007">AS423</f>
         <v>0.46</v>
       </c>
       <c r="AT439" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU439" s="138">
         <v>0.24</v>
       </c>
       <c r="AV439" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW439" s="38">
@@ -87378,31 +87359,30 @@
         <v>114</v>
       </c>
       <c r="BF439" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG439" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH439" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI439" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ439" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ439" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK439" s="138" t="str">
-        <f t="shared" ref="BK439:BL439" si="1010">BK423</f>
+        <f t="shared" ref="BK439:BL439" si="1008">BK423</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL439" s="138" t="str">
-        <f t="shared" si="1010"/>
+        <f t="shared" si="1008"/>
         <v>T24-2022 ExtWall 8in Conc U=0.253</v>
       </c>
       <c r="BM439" s="2" t="s">
@@ -87445,23 +87425,23 @@
         <v>274</v>
       </c>
       <c r="BZ439" s="124" t="str">
-        <f t="shared" ref="BZ439:CD439" si="1011">BZ438</f>
+        <f t="shared" ref="BZ439:CD439" si="1009">BZ438</f>
         <v>not compact</v>
       </c>
       <c r="CA439" s="69" t="str">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>not compact</v>
       </c>
       <c r="CB439" s="35" t="str">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC439" s="35" t="str">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>Standard</v>
       </c>
       <c r="CD439" s="40">
-        <f t="shared" si="1011"/>
+        <f t="shared" si="1009"/>
         <v>-1</v>
       </c>
       <c r="CE439" s="40">
@@ -87491,11 +87471,11 @@
         <v>13</v>
       </c>
       <c r="D440" s="35">
-        <f t="shared" ref="D440:E440" si="1012">D439</f>
+        <f t="shared" ref="D440:E440" si="1010">D439</f>
         <v>2025</v>
       </c>
       <c r="E440" s="40" t="str">
-        <f t="shared" si="1012"/>
+        <f t="shared" si="1010"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F440" s="2">
@@ -87541,7 +87521,7 @@
         <v>0.62</v>
       </c>
       <c r="T440" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U440" s="38">
@@ -87563,22 +87543,22 @@
         <v>15</v>
       </c>
       <c r="AA440" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB440" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC440" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD440" s="120">
-        <f t="shared" ref="AD440:AE440" si="1013">AD424</f>
+        <f t="shared" ref="AD440:AE440" si="1011">AD424</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE440" s="120">
-        <f t="shared" si="1013"/>
+        <f t="shared" si="1011"/>
         <v>0.21099999999999999</v>
       </c>
       <c r="AF440" s="2">
@@ -87609,33 +87589,33 @@
         <v>5016</v>
       </c>
       <c r="AO440" s="40">
-        <f t="shared" ref="AO440:AP440" si="1014">AO439</f>
+        <f t="shared" ref="AO440:AP440" si="1012">AO439</f>
         <v>0.7</v>
       </c>
       <c r="AP440" s="40" t="str">
-        <f t="shared" si="1014"/>
+        <f t="shared" si="1012"/>
         <v>Yes</v>
       </c>
       <c r="AQ440" s="138">
-        <f t="shared" ref="AQ440:AS440" si="1015">AQ424</f>
+        <f t="shared" ref="AQ440" si="1013">AQ424</f>
         <v>0.41</v>
       </c>
       <c r="AR440" s="138">
         <v>0.26</v>
       </c>
       <c r="AS440" s="138">
-        <f t="shared" ref="AS440:AU440" si="1016">AS424</f>
+        <f t="shared" ref="AS440" si="1014">AS424</f>
         <v>0.46</v>
       </c>
       <c r="AT440" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU440" s="138">
         <v>0.24</v>
       </c>
       <c r="AV440" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW440" s="38">
@@ -87666,31 +87646,30 @@
         <v>114</v>
       </c>
       <c r="BF440" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG440" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH440" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.059</v>
       </c>
       <c r="BI440" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ440" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ440" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK440" s="138" t="str">
-        <f t="shared" ref="BK440:BL440" si="1017">BK424</f>
+        <f t="shared" ref="BK440:BL440" si="1015">BK424</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL440" s="138" t="str">
-        <f t="shared" si="1017"/>
+        <f t="shared" si="1015"/>
         <v>T24-2022 ExtWall 8in Conc U=0.211</v>
       </c>
       <c r="BM440" s="2" t="s">
@@ -87733,23 +87712,23 @@
         <v>274</v>
       </c>
       <c r="BZ440" s="124" t="str">
-        <f t="shared" ref="BZ440:CD440" si="1018">BZ439</f>
+        <f t="shared" ref="BZ440:CD440" si="1016">BZ439</f>
         <v>not compact</v>
       </c>
       <c r="CA440" s="69" t="str">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>not compact</v>
       </c>
       <c r="CB440" s="35" t="str">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC440" s="35" t="str">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>Standard</v>
       </c>
       <c r="CD440" s="40">
-        <f t="shared" si="1018"/>
+        <f t="shared" si="1016"/>
         <v>-1</v>
       </c>
       <c r="CE440" s="40">
@@ -87779,11 +87758,11 @@
         <v>14</v>
       </c>
       <c r="D441" s="35">
-        <f t="shared" ref="D441:E441" si="1019">D440</f>
+        <f t="shared" ref="D441:E441" si="1017">D440</f>
         <v>2025</v>
       </c>
       <c r="E441" s="40" t="str">
-        <f t="shared" si="1019"/>
+        <f t="shared" si="1017"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F441" s="2">
@@ -87829,7 +87808,7 @@
         <v>0.62</v>
       </c>
       <c r="T441" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U441" s="38">
@@ -87851,22 +87830,22 @@
         <v>15</v>
       </c>
       <c r="AA441" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB441" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC441" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD441" s="120">
-        <f t="shared" ref="AD441:AE441" si="1020">AD425</f>
+        <f t="shared" ref="AD441:AE441" si="1018">AD425</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE441" s="120">
-        <f t="shared" si="1020"/>
+        <f t="shared" si="1018"/>
         <v>0.184</v>
       </c>
       <c r="AF441" s="2">
@@ -87897,33 +87876,33 @@
         <v>5016</v>
       </c>
       <c r="AO441" s="40">
-        <f t="shared" ref="AO441:AP441" si="1021">AO440</f>
+        <f t="shared" ref="AO441:AP441" si="1019">AO440</f>
         <v>0.7</v>
       </c>
       <c r="AP441" s="40" t="str">
-        <f t="shared" si="1021"/>
+        <f t="shared" si="1019"/>
         <v>Yes</v>
       </c>
       <c r="AQ441" s="138">
-        <f t="shared" ref="AQ441:AS441" si="1022">AQ425</f>
+        <f t="shared" ref="AQ441" si="1020">AQ425</f>
         <v>0.41</v>
       </c>
       <c r="AR441" s="138">
         <v>0.25</v>
       </c>
       <c r="AS441" s="138">
-        <f t="shared" ref="AS441:AU441" si="1023">AS425</f>
+        <f t="shared" ref="AS441" si="1021">AS425</f>
         <v>0.46</v>
       </c>
       <c r="AT441" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU441" s="138">
         <v>0.24</v>
       </c>
       <c r="AV441" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW441" s="38">
@@ -87954,31 +87933,30 @@
         <v>114</v>
       </c>
       <c r="BF441" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG441" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH441" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI441" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ441" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ441" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK441" s="138" t="str">
-        <f t="shared" ref="BK441:BL441" si="1024">BK425</f>
+        <f t="shared" ref="BK441:BL441" si="1022">BK425</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL441" s="138" t="str">
-        <f t="shared" si="1024"/>
+        <f t="shared" si="1022"/>
         <v>T24-2022 ExtWall 8in Conc U=0.184</v>
       </c>
       <c r="BM441" s="2" t="s">
@@ -88021,23 +87999,23 @@
         <v>274</v>
       </c>
       <c r="BZ441" s="124" t="str">
-        <f t="shared" ref="BZ441:CD441" si="1025">BZ440</f>
+        <f t="shared" ref="BZ441:CD441" si="1023">BZ440</f>
         <v>not compact</v>
       </c>
       <c r="CA441" s="69" t="str">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>not compact</v>
       </c>
       <c r="CB441" s="35" t="str">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC441" s="35" t="str">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>Standard</v>
       </c>
       <c r="CD441" s="40">
-        <f t="shared" si="1025"/>
+        <f t="shared" si="1023"/>
         <v>-1</v>
       </c>
       <c r="CE441" s="40">
@@ -88067,11 +88045,11 @@
         <v>15</v>
       </c>
       <c r="D442" s="35">
-        <f t="shared" ref="D442:E442" si="1026">D441</f>
+        <f t="shared" ref="D442:E442" si="1024">D441</f>
         <v>2025</v>
       </c>
       <c r="E442" s="40" t="str">
-        <f t="shared" si="1026"/>
+        <f t="shared" si="1024"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F442" s="2">
@@ -88117,7 +88095,7 @@
         <v>0.62</v>
       </c>
       <c r="T442" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U442" s="38">
@@ -88139,22 +88117,22 @@
         <v>15</v>
       </c>
       <c r="AA442" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB442" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC442" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD442" s="120">
-        <f t="shared" ref="AD442:AE442" si="1027">AD426</f>
+        <f t="shared" ref="AD442:AE442" si="1025">AD426</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AE442" s="120">
-        <f t="shared" si="1027"/>
+        <f t="shared" si="1025"/>
         <v>0.184</v>
       </c>
       <c r="AF442" s="2">
@@ -88185,33 +88163,33 @@
         <v>5016</v>
       </c>
       <c r="AO442" s="40">
-        <f t="shared" ref="AO442:AP442" si="1028">AO441</f>
+        <f t="shared" ref="AO442:AP442" si="1026">AO441</f>
         <v>0.7</v>
       </c>
       <c r="AP442" s="40" t="str">
-        <f t="shared" si="1028"/>
+        <f t="shared" si="1026"/>
         <v>Yes</v>
       </c>
       <c r="AQ442" s="138">
-        <f t="shared" ref="AQ442:AS442" si="1029">AQ426</f>
+        <f t="shared" ref="AQ442" si="1027">AQ426</f>
         <v>0.41</v>
       </c>
       <c r="AR442" s="138">
         <v>0.26</v>
       </c>
       <c r="AS442" s="138">
-        <f t="shared" ref="AS442:AU442" si="1030">AS426</f>
+        <f t="shared" ref="AS442" si="1028">AS426</f>
         <v>0.46</v>
       </c>
       <c r="AT442" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.4</v>
       </c>
       <c r="AU442" s="138">
         <v>0.24</v>
       </c>
       <c r="AV442" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW442" s="38">
@@ -88242,31 +88220,30 @@
         <v>114</v>
       </c>
       <c r="BF442" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG442" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH442" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI442" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ442" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ442" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK442" s="138" t="str">
-        <f t="shared" ref="BK442:BL442" si="1031">BK426</f>
+        <f t="shared" ref="BK442:BL442" si="1029">BK426</f>
         <v>T24-2022 ExtWall 6in Conc R13</v>
       </c>
       <c r="BL442" s="138" t="str">
-        <f t="shared" si="1031"/>
+        <f t="shared" si="1029"/>
         <v>T24-2022 ExtWall 8in Conc U=0.184</v>
       </c>
       <c r="BM442" s="2" t="s">
@@ -88309,23 +88286,23 @@
         <v>274</v>
       </c>
       <c r="BZ442" s="124" t="str">
-        <f t="shared" ref="BZ442:CD442" si="1032">BZ441</f>
+        <f t="shared" ref="BZ442:CD442" si="1030">BZ441</f>
         <v>not compact</v>
       </c>
       <c r="CA442" s="69" t="str">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>not compact</v>
       </c>
       <c r="CB442" s="35" t="str">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC442" s="35" t="str">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>Standard</v>
       </c>
       <c r="CD442" s="40">
-        <f t="shared" si="1032"/>
+        <f t="shared" si="1030"/>
         <v>-1</v>
       </c>
       <c r="CE442" s="40">
@@ -88355,11 +88332,11 @@
         <v>16</v>
       </c>
       <c r="D443" s="35">
-        <f t="shared" ref="D443:E443" si="1033">D442</f>
+        <f t="shared" ref="D443:E443" si="1031">D442</f>
         <v>2025</v>
       </c>
       <c r="E443" s="40" t="str">
-        <f t="shared" si="1033"/>
+        <f t="shared" si="1031"/>
         <v>HiRiseRes</v>
       </c>
       <c r="F443" s="2">
@@ -88405,7 +88382,7 @@
         <v>0.62</v>
       </c>
       <c r="T443" s="35">
-        <f t="shared" si="939"/>
+        <f t="shared" si="938"/>
         <v>7</v>
       </c>
       <c r="U443" s="38">
@@ -88427,22 +88404,22 @@
         <v>15</v>
       </c>
       <c r="AA443" s="2">
-        <f t="shared" si="934"/>
+        <f t="shared" si="933"/>
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="AB443" s="2">
-        <f t="shared" si="929"/>
+        <f t="shared" si="928"/>
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AC443" s="120">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="AD443" s="120">
-        <f t="shared" ref="AD443:AE443" si="1034">AD427</f>
+        <f t="shared" ref="AD443:AE443" si="1032">AD427</f>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AE443" s="120">
-        <f t="shared" si="1034"/>
+        <f t="shared" si="1032"/>
         <v>0.16</v>
       </c>
       <c r="AF443" s="2">
@@ -88473,33 +88450,33 @@
         <v>10016</v>
       </c>
       <c r="AO443" s="40">
-        <f t="shared" ref="AO443:AP443" si="1035">AO442</f>
+        <f t="shared" ref="AO443:AP443" si="1033">AO442</f>
         <v>0.7</v>
       </c>
       <c r="AP443" s="40" t="str">
-        <f t="shared" si="1035"/>
+        <f t="shared" si="1033"/>
         <v>Yes</v>
       </c>
       <c r="AQ443" s="138">
-        <f t="shared" ref="AQ443:AS443" si="1036">AQ427</f>
+        <f t="shared" ref="AQ443" si="1034">AQ427</f>
         <v>0.38</v>
       </c>
       <c r="AR443" s="138">
         <v>0.25</v>
       </c>
       <c r="AS443" s="138">
-        <f t="shared" ref="AS443:AU443" si="1037">AS427</f>
+        <f t="shared" ref="AS443" si="1035">AS427</f>
         <v>0.46</v>
       </c>
       <c r="AT443" s="138">
-        <f t="shared" si="943"/>
+        <f t="shared" si="942"/>
         <v>0.38</v>
       </c>
       <c r="AU443" s="138">
         <v>0.24</v>
       </c>
       <c r="AV443" s="138">
-        <f t="shared" si="944"/>
+        <f t="shared" si="943"/>
         <v>0.37</v>
       </c>
       <c r="AW443" s="38">
@@ -88530,31 +88507,30 @@
         <v>114</v>
       </c>
       <c r="BF443" s="40">
-        <f t="shared" si="945"/>
+        <f t="shared" si="944"/>
         <v>0</v>
       </c>
       <c r="BG443" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.057</v>
       </c>
       <c r="BH443" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
       <c r="BI443" s="138" t="str">
-        <f t="shared" si="936"/>
+        <f t="shared" si="935"/>
         <v>T24-2022 ExtWall 2x6 16oc U=0.051</v>
       </c>
-      <c r="BJ443" s="35" t="str">
-        <f t="shared" si="946"/>
-        <v>T24-2019 IntWall 2x6 16oc R21</v>
+      <c r="BJ443" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="BK443" s="138" t="str">
-        <f t="shared" ref="BK443:BL443" si="1038">BK427</f>
+        <f t="shared" ref="BK443:BL443" si="1036">BK427</f>
         <v>T24-2022 ExtWall 6in Conc R17</v>
       </c>
       <c r="BL443" s="138" t="str">
-        <f t="shared" si="1038"/>
+        <f t="shared" si="1036"/>
         <v>T24-2022 ExtWall 10in Conc U=0.160</v>
       </c>
       <c r="BM443" s="2" t="s">
@@ -88597,23 +88573,23 @@
         <v>274</v>
       </c>
       <c r="BZ443" s="124" t="str">
-        <f t="shared" ref="BZ443:CD443" si="1039">BZ442</f>
+        <f t="shared" ref="BZ443:CD443" si="1037">BZ442</f>
         <v>not compact</v>
       </c>
       <c r="CA443" s="69" t="str">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>not compact</v>
       </c>
       <c r="CB443" s="35" t="str">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>Pipe Insulation, All Lines</v>
       </c>
       <c r="CC443" s="35" t="str">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>Standard</v>
       </c>
       <c r="CD443" s="40">
-        <f t="shared" si="1039"/>
+        <f t="shared" si="1037"/>
         <v>-1</v>
       </c>
       <c r="CE443" s="121">

</xml_diff>